<commit_message>
added templates for terms and conditions
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP_REPO\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9B89D4-9D0B-472A-B528-7A4CF81A2944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="500"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11380" uniqueCount="1903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11578" uniqueCount="1927">
   <si>
     <t>id</t>
   </si>
@@ -15361,11 +15362,137 @@
   <si>
     <t>reg-android-preview-template-part</t>
   </si>
+  <si>
+    <t>Order a physical card</t>
+  </si>
+  <si>
+    <t>tnc-order-a-physical-card</t>
+  </si>
+  <si>
+    <t>Share your credential with a partner</t>
+  </si>
+  <si>
+    <t>tnc-share-cred-with-partner</t>
+  </si>
+  <si>
+    <t>Update demographic data</t>
+  </si>
+  <si>
+    <t>tnc-update-demo</t>
+  </si>
+  <si>
+    <t>1. Your chosen data will be shared with the chosen third party (print partner).
+ 2. You are responsible for any and all costs and fees associated with agreements entered into with the third-party provider.
+ 3. The delivery of the printed card will be the sole responsibility of the partner.
+ 4. Under no circumstances will we be liable for loss or misuse of data whatsoever, arising from the usage of data shared with the partner.
+ 5. If a third-party provider ceases to make its service available or requires MOSIP to suspend or terminate the provision of all or any part of its services to you that part of data or services will be terminated immediately without notice or further obligation to you.</t>
+  </si>
+  <si>
+    <t>1. ستتم مشاركة البيانات التي اخترتها مع الطرف الثالث المختار (شريك الطباعة).
+ 2. أنت مسؤول عن أي وجميع التكاليف والرسوم المرتبطة بالاتفاقيات المبرمة مع مزود الطرف الثالث.
+ 3. تسليم البطاقة المطبوعة سيكون من مسؤولية الشريك وحده.
+ 4. لن نتحمل تحت أي ظرف من الظروف المسؤولية عن فقدان البيانات أو إساءة استخدامها على الإطلاق ، الناشئة عن استخدام البيانات التي تمت مشاركتها مع الشريك.
+ 5. إذا توقف موفر الطرف الثالث عن إتاحة خدمته أو طلب من MOSIP تعليق أو إنهاء توفير كل أو أي جزء من خدماته لك ، فسيتم إنهاء هذا الجزء من البيانات أو الخدمات على الفور دون إشعار أو التزام آخر تجاهك .</t>
+  </si>
+  <si>
+    <t>1. Vos données choisies seront partagées avec le tiers choisi (partenaire d'impression).
+ 2. Vous êtes responsable de tous les coûts et frais associés aux accords conclus avec le fournisseur tiers.
+ 3. La livraison de la carte imprimée sera de la seule responsabilité du partenaire.
+ 4. Nous ne serons en aucun cas responsables de la perte ou de l'utilisation abusive des données, quelle qu'elle soit, résultant de l'utilisation des données partagées avec le partenaire.
+ 5. Si un fournisseur tiers cesse de mettre son service à disposition ou exige que MOSIP suspende ou résilie la fourniture de tout ou partie de ses services, cette partie des données ou des services sera immédiatement résiliée sans préavis ni autre obligation envers vous. .</t>
+  </si>
+  <si>
+    <t>1. आपका चुना हुआ डेटा चुने हुए तीसरे पक्ष (प्रिंट पार्टनर) के साथ साझा किया जाएगा।
+ 2. आप तृतीय-पक्ष प्रदाता के साथ किए गए समझौतों से जुड़ी किसी भी और सभी लागतों और शुल्क के लिए जिम्मेदार हैं।
+ 3. मुद्रित कार्ड की सुपुर्दगी की एकमात्र जिम्मेदारी भागीदार की होगी।
+ 4. पार्टनर के साथ साझा किए गए डेटा के उपयोग से उत्पन्न होने वाले डेटा के नुकसान या दुरुपयोग के लिए हम किसी भी परिस्थिति में उत्तरदायी नहीं होंगे।
+ 5. यदि कोई तृतीय-पक्ष प्रदाता अपनी सेवा उपलब्ध कराना बंद कर देता है या MOSIP को आपकी सेवाओं के सभी या किसी भी हिस्से के प्रावधान को निलंबित या समाप्त करने की आवश्यकता होती है, तो डेटा या सेवाओं का वह हिस्सा बिना किसी सूचना या आपके लिए आगे की बाध्यता के तुरंत समाप्त कर दिया जाएगा। ।</t>
+  </si>
+  <si>
+    <t>1. ನಿಮ್ಮ ಆಯ್ಕೆಮಾಡಿದ ಡೇಟಾವನ್ನು ಆಯ್ಕೆಮಾಡಿದ ಮೂರನೇ ವ್ಯಕ್ತಿಯೊಂದಿಗೆ ಹಂಚಿಕೊಳ್ಳಲಾಗುತ್ತದೆ (ಮುದ್ರಣ ಪಾಲುದಾರ).
+ 2. ಮೂರನೇ ವ್ಯಕ್ತಿಯ ಪೂರೈಕೆದಾರರೊಂದಿಗೆ ಮಾಡಿಕೊಂಡಿರುವ ಒಪ್ಪಂದಗಳಿಗೆ ಸಂಬಂಧಿಸಿದ ಯಾವುದೇ ಮತ್ತು ಎಲ್ಲಾ ವೆಚ್ಚಗಳು ಮತ್ತು ಶುಲ್ಕಗಳಿಗೆ ನೀವು ಜವಾಬ್ದಾರರಾಗಿರುತ್ತೀರಿ.
+ 3. ಮುದ್ರಿತ ಕಾರ್ಡ್‌ನ ವಿತರಣೆಯು ಪಾಲುದಾರರ ಸಂಪೂರ್ಣ ಜವಾಬ್ದಾರಿಯಾಗಿರುತ್ತದೆ.
+ 4. ಪಾಲುದಾರರೊಂದಿಗೆ ಹಂಚಿಕೊಂಡ ಡೇಟಾದ ಬಳಕೆಯಿಂದ ಉಂಟಾಗುವ ಡೇಟಾದ ನಷ್ಟ ಅಥವಾ ದುರ್ಬಳಕೆಗೆ ನಾವು ಯಾವುದೇ ಸಂದರ್ಭಗಳಲ್ಲಿ ಜವಾಬ್ದಾರರಾಗಿರುವುದಿಲ್ಲ.
+ 5. ಥರ್ಡ್-ಪಾರ್ಟಿ ಪ್ರೊವೈಡರ್ ತನ್ನ ಸೇವೆಯನ್ನು ಲಭ್ಯವಾಗುವಂತೆ ಮಾಡುವುದನ್ನು ನಿಲ್ಲಿಸಿದರೆ ಅಥವಾ MOSIP ನಿಮಗೆ ಅದರ ಎಲ್ಲಾ ಅಥವಾ ಯಾವುದೇ ಭಾಗದ ಸೇವೆಗಳ ನಿಬಂಧನೆಯನ್ನು ಅಮಾನತುಗೊಳಿಸಲು ಅಥವಾ ಅಂತ್ಯಗೊಳಿಸಲು ಅಗತ್ಯವಿದ್ದರೆ ಡೇಟಾ ಅಥವಾ ಸೇವೆಗಳ ಭಾಗವನ್ನು ನಿಮಗೆ ಸೂಚನೆ ಅಥವಾ ಹೆಚ್ಚಿನ ಬಾಧ್ಯತೆ ಇಲ್ಲದೆ ತಕ್ಷಣವೇ ಕೊನೆಗೊಳಿಸಲಾಗುತ್ತದೆ .</t>
+  </si>
+  <si>
+    <t>1. நீங்கள் தேர்ந்தெடுத்த தரவு தேர்ந்தெடுக்கப்பட்ட மூன்றாம் தரப்பினருடன் (அச்சு பார்ட்னர்) பகிரப்படும்.
+ 2. மூன்றாம் தரப்பு வழங்குனருடன் செய்துகொள்ளப்பட்ட ஒப்பந்தங்களுடன் தொடர்புடைய அனைத்து செலவுகள் மற்றும் கட்டணங்களுக்கு நீங்கள் பொறுப்பாவீர்கள்.
+ 3. அச்சிடப்பட்ட அட்டையை வழங்குவது பங்குதாரரின் முழுப் பொறுப்பாகும்.
+ 4. கூட்டாளருடன் பகிரப்பட்ட தரவைப் பயன்படுத்துவதால் ஏற்படும் தரவு இழப்பு அல்லது தவறான பயன்பாட்டிற்கு எந்தச் சூழ்நிலையிலும் நாங்கள் பொறுப்பாக மாட்டோம்.
+ 5. ஒரு மூன்றாம் தரப்பு வழங்குநர் தனது சேவையை வழங்குவதை நிறுத்தினால் அல்லது MOSIP ஆனது அதன் அனைத்து அல்லது எந்தப் பகுதியையும் உங்களுக்கு வழங்குவதை இடைநிறுத்தவோ அல்லது நிறுத்தவோ தேவைப்பட்டால், தரவு அல்லது சேவைகளின் ஒரு பகுதி உங்களுக்கு அறிவிப்பு அல்லது கூடுதல் பொறுப்பு இல்லாமல் உடனடியாக நிறுத்தப்படும். .</t>
+  </si>
+  <si>
+    <t>1. Your data will be shared with the chosen third party (credential partner)
+ 2. You are responsible for any and all costs and fees associated with agreements entered into with the third-party provider.
+ 3. Under no circumstances will we be liable for loss or misuse of data whatsoever, arising from the usage of data shared with the partner.
+ 4. If a third-party provider ceases to make its service available or requires MOSIP to suspend or terminate the provision of all or any part of its services to you that part of data or services will be terminated immediately without notice or further obligation to you.</t>
+  </si>
+  <si>
+    <t>1. ستتم مشاركة بياناتك مع الطرف الثالث المختار (الشريك المعتمد)
+ 2. أنت مسؤول عن أي وجميع التكاليف والرسوم المرتبطة بالاتفاقيات المبرمة مع مزود الطرف الثالث.
+ 3. لن نتحمل تحت أي ظرف من الظروف المسؤولية عن فقدان البيانات أو إساءة استخدامها على الإطلاق ، الناشئة عن استخدام البيانات التي تمت مشاركتها مع الشريك.
+ 4. إذا توقف موفر الطرف الثالث عن إتاحة خدمته أو طلب من MOSIP تعليق أو إنهاء توفير كل أو أي جزء من خدماته لك ، فسيتم إنهاء هذا الجزء من البيانات أو الخدمات على الفور دون إشعار أو التزام آخر تجاهك .</t>
+  </si>
+  <si>
+    <t>1. Vos données seront partagées avec le tiers choisi (partenaire d'identification)
+ 2. Vous êtes responsable de tous les coûts et frais associés aux accords conclus avec le fournisseur tiers.
+ 3. Nous ne serons en aucun cas responsables de la perte ou de l'utilisation abusive des données, quelle qu'elle soit, résultant de l'utilisation des données partagées avec le partenaire.
+ 4. Si un fournisseur tiers cesse de mettre son service à disposition ou exige que MOSIP suspende ou résilie la fourniture de tout ou partie de ses services, cette partie des données ou des services sera immédiatement résiliée sans préavis ni autre obligation envers vous. .</t>
+  </si>
+  <si>
+    <t>1. आपका डेटा चुने हुए तीसरे पक्ष (क्रेडेंशियल पार्टनर) के साथ साझा किया जाएगा
+ 2. आप तृतीय-पक्ष प्रदाता के साथ किए गए समझौतों से जुड़ी किसी भी और सभी लागतों और शुल्क के लिए जिम्मेदार हैं।
+ 3. पार्टनर के साथ साझा किए गए डेटा के उपयोग से उत्पन्न होने वाले डेटा के नुकसान या दुरुपयोग के लिए हम किसी भी परिस्थिति में उत्तरदायी नहीं होंगे।
+ 4. यदि कोई तृतीय-पक्ष प्रदाता अपनी सेवा उपलब्ध कराना बंद कर देता है या MOSIP को आपकी सेवाओं के सभी या किसी भी हिस्से के प्रावधान को निलंबित या समाप्त करने की आवश्यकता होती है, तो डेटा या सेवाओं का वह हिस्सा बिना किसी सूचना या आपके लिए आगे की बाध्यता के तुरंत समाप्त कर दिया जाएगा। ।</t>
+  </si>
+  <si>
+    <t>1. ನಿಮ್ಮ ಡೇಟಾವನ್ನು ಆಯ್ಕೆ ಮಾಡಿದ ಮೂರನೇ ವ್ಯಕ್ತಿಯೊಂದಿಗೆ ಹಂಚಿಕೊಳ್ಳಲಾಗುತ್ತದೆ (ರುಜುವಾತು ಪಾಲುದಾರ)
+ 2. ಮೂರನೇ ವ್ಯಕ್ತಿಯ ಪೂರೈಕೆದಾರರೊಂದಿಗೆ ಮಾಡಿಕೊಂಡಿರುವ ಒಪ್ಪಂದಗಳಿಗೆ ಸಂಬಂಧಿಸಿದ ಯಾವುದೇ ಮತ್ತು ಎಲ್ಲಾ ವೆಚ್ಚಗಳು ಮತ್ತು ಶುಲ್ಕಗಳಿಗೆ ನೀವು ಜವಾಬ್ದಾರರಾಗಿರುತ್ತೀರಿ.
+ 3. ಪಾಲುದಾರರೊಂದಿಗೆ ಹಂಚಿಕೊಂಡ ಡೇಟಾದ ಬಳಕೆಯಿಂದ ಉಂಟಾಗುವ ಡೇಟಾದ ನಷ್ಟ ಅಥವಾ ದುರುಪಯೋಗಕ್ಕೆ ನಾವು ಯಾವುದೇ ಸಂದರ್ಭಗಳಲ್ಲಿ ಜವಾಬ್ದಾರರಾಗಿರುವುದಿಲ್ಲ.
+ 4. ಥರ್ಡ್-ಪಾರ್ಟಿ ಪ್ರೊವೈಡರ್ ತನ್ನ ಸೇವೆಯನ್ನು ಲಭ್ಯವಾಗುವಂತೆ ಮಾಡುವುದನ್ನು ನಿಲ್ಲಿಸಿದರೆ ಅಥವಾ MOSIP ನಿಮಗೆ ಅದರ ಎಲ್ಲಾ ಅಥವಾ ಯಾವುದೇ ಭಾಗದ ಸೇವೆಗಳ ನಿಬಂಧನೆಯನ್ನು ಅಮಾನತುಗೊಳಿಸಲು ಅಥವಾ ಅಂತ್ಯಗೊಳಿಸಲು ಅಗತ್ಯವಿದ್ದರೆ ಡೇಟಾ ಅಥವಾ ಸೇವೆಗಳ ಭಾಗವನ್ನು ತಕ್ಷಣವೇ ನಿಮಗೆ ಸೂಚನೆ ಅಥವಾ ಹೆಚ್ಚಿನ ಬಾಧ್ಯತೆ ಇಲ್ಲದೆ ಕೊನೆಗೊಳಿಸಲಾಗುತ್ತದೆ .</t>
+  </si>
+  <si>
+    <t>1. உங்கள் தரவு தேர்ந்தெடுக்கப்பட்ட மூன்றாம் தரப்பினருடன் (நற்சான்றிதழ் கூட்டாளர்) பகிரப்படும்
+ 2. மூன்றாம் தரப்பு வழங்குனருடன் செய்துகொள்ளப்பட்ட ஒப்பந்தங்களுடன் தொடர்புடைய அனைத்து செலவுகள் மற்றும் கட்டணங்களுக்கு நீங்கள் பொறுப்பாவீர்கள்.
+ 3. கூட்டாளருடன் பகிரப்பட்ட தரவைப் பயன்படுத்துவதால் ஏற்படும் தரவு இழப்பு அல்லது தவறான பயன்பாட்டிற்கு எந்தச் சூழ்நிலையிலும் நாங்கள் பொறுப்பேற்க மாட்டோம்.
+ 4. ஒரு மூன்றாம் தரப்பு வழங்குநர் தனது சேவையை வழங்குவதை நிறுத்தினால் அல்லது MOSIP ஆனது அதன் அனைத்து அல்லது எந்தப் பகுதியையும் உங்களுக்கு வழங்குவதை இடைநிறுத்தவோ அல்லது நிறுத்தவோ தேவைப்பட்டால், தரவு அல்லது சேவைகளின் ஒரு பகுதி உங்களுக்கு அறிவிப்பு அல்லது கூடுதல் பொறுப்பு இல்லாமல் உடனடியாக நிறுத்தப்படும். .</t>
+  </si>
+  <si>
+    <t>1. The data chosen by you will be updated after the Proof of address or Proof of Identity is duly verified.
+ 2. You are responsible for any and all costs and fees associated with an agreement to update your data.
+ 3. You are responsible for any changes made to your already existing personal data or uploaded document to support the same.</t>
+  </si>
+  <si>
+    <t>1. سيتم تحديث البيانات التي اخترتها بعد التحقق من إثبات العنوان أو إثبات الهوية على النحو الواجب.
+ 2. أنت مسؤول عن أي وجميع التكاليف والرسوم المرتبطة باتفاقية لتحديث بياناتك.
+ 3. أنت مسؤول عن أي تغييرات يتم إجراؤها على بياناتك الشخصية الموجودة بالفعل أو المستند الذي تم تحميله لدعمها ".</t>
+  </si>
+  <si>
+    <t>1. Les données que vous avez choisies seront mises à jour après que le justificatif de domicile ou la preuve d'identité aura été dûment vérifié.
+ 2. Vous êtes responsable de tous les coûts et frais associés à un accord de mise à jour de vos données.
+ 3. Vous êtes responsable de toute modification apportée à vos données personnelles déjà existantes ou à un document téléchargé pour les prendre en charge.</t>
+  </si>
+  <si>
+    <t>1. आपके द्वारा चुने गए डेटा को पते के प्रमाण या पहचान के प्रमाण के विधिवत सत्यापित होने के बाद अपडेट किया जाएगा।
+ 2. आप अपने डेटा को अपडेट करने के लिए एक समझौते से जुड़े किसी भी और सभी लागतों और शुल्क के लिए जिम्मेदार हैं।
+ 3. आप अपने पहले से मौजूद व्यक्तिगत डेटा या उसके समर्थन के लिए अपलोड किए गए दस्तावेज़ में किए गए किसी भी बदलाव के लिए जिम्मेदार हैं।</t>
+  </si>
+  <si>
+    <t>1. ವಿಳಾಸದ ಪುರಾವೆ ಅಥವಾ ಗುರುತಿನ ಪುರಾವೆಯನ್ನು ಸರಿಯಾಗಿ ಪರಿಶೀಲಿಸಿದ ನಂತರ ನೀವು ಆಯ್ಕೆ ಮಾಡಿದ ಡೇಟಾವನ್ನು ನವೀಕರಿಸಲಾಗುತ್ತದೆ.
+ 2. ನಿಮ್ಮ ಡೇಟಾವನ್ನು ನವೀಕರಿಸಲು ಒಪ್ಪಂದಕ್ಕೆ ಸಂಬಂಧಿಸಿದ ಯಾವುದೇ ಮತ್ತು ಎಲ್ಲಾ ವೆಚ್ಚಗಳು ಮತ್ತು ಶುಲ್ಕಗಳಿಗೆ ನೀವು ಜವಾಬ್ದಾರರಾಗಿರುತ್ತೀರಿ.
+ 3. ನಿಮ್ಮ ಈಗಾಗಲೇ ಅಸ್ತಿತ್ವದಲ್ಲಿರುವ ವೈಯಕ್ತಿಕ ಡೇಟಾ ಅಥವಾ ಅದನ್ನು ಬೆಂಬಲಿಸಲು ಅಪ್‌ಲೋಡ್ ಮಾಡಿದ ಡಾಕ್ಯುಮೆಂಟ್‌ಗೆ ಮಾಡಿದ ಯಾವುದೇ ಬದಲಾವಣೆಗಳಿಗೆ ನೀವು ಜವಾಬ್ದಾರರಾಗಿರುತ್ತೀರಿ.</t>
+  </si>
+  <si>
+    <t>1. நீங்கள் தேர்ந்தெடுத்த தரவு முகவரிச் சான்று அல்லது அடையாளச் சான்று முறையாகச் சரிபார்க்கப்பட்ட பிறகு புதுப்பிக்கப்படும்.
+ 2. உங்கள் தரவைப் புதுப்பிப்பதற்கான ஒப்பந்தத்துடன் தொடர்புடைய அனைத்து செலவுகள் மற்றும் கட்டணங்களுக்கு நீங்கள் பொறுப்பாவீர்கள்.
+ 3. ஏற்கனவே உள்ள உங்கள் தனிப்பட்ட தரவு அல்லது பதிவேற்றிய ஆவணத்தில் ஏதேனும் மாற்றங்கள் செய்யப்பட்டால் அதற்கு நீங்களே பொறுப்பு.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -15502,7 +15629,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -15814,11 +15941,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M950"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A939" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A948" sqref="A948:M950"/>
+    <sheetView tabSelected="1" topLeftCell="D968" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E971" sqref="E971"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -54774,6 +54901,744 @@
         <v>23</v>
       </c>
     </row>
+    <row r="951" spans="1:13" ht="240">
+      <c r="A951">
+        <v>1244</v>
+      </c>
+      <c r="B951" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C951" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D951" t="s">
+        <v>15</v>
+      </c>
+      <c r="E951" t="s">
+        <v>16</v>
+      </c>
+      <c r="F951" s="16" t="s">
+        <v>1909</v>
+      </c>
+      <c r="G951">
+        <v>10006</v>
+      </c>
+      <c r="H951" t="s">
+        <v>404</v>
+      </c>
+      <c r="I951" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J951" t="s">
+        <v>20</v>
+      </c>
+      <c r="K951" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L951" t="s">
+        <v>22</v>
+      </c>
+      <c r="M951" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="952" spans="1:13" ht="180">
+      <c r="A952">
+        <v>1244</v>
+      </c>
+      <c r="B952" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C952" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D952" t="s">
+        <v>15</v>
+      </c>
+      <c r="E952" t="s">
+        <v>16</v>
+      </c>
+      <c r="F952" s="16" t="s">
+        <v>1910</v>
+      </c>
+      <c r="G952">
+        <v>10006</v>
+      </c>
+      <c r="H952" t="s">
+        <v>404</v>
+      </c>
+      <c r="I952" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J952" t="s">
+        <v>43</v>
+      </c>
+      <c r="K952" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L952" t="s">
+        <v>22</v>
+      </c>
+      <c r="M952" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="953" spans="1:13" ht="240">
+      <c r="A953">
+        <v>1244</v>
+      </c>
+      <c r="B953" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C953" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D953" t="s">
+        <v>15</v>
+      </c>
+      <c r="E953" t="s">
+        <v>16</v>
+      </c>
+      <c r="F953" s="16" t="s">
+        <v>1911</v>
+      </c>
+      <c r="G953">
+        <v>10006</v>
+      </c>
+      <c r="H953" t="s">
+        <v>404</v>
+      </c>
+      <c r="I953" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J953" t="s">
+        <v>35</v>
+      </c>
+      <c r="K953" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L953" t="s">
+        <v>22</v>
+      </c>
+      <c r="M953" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="954" spans="1:13" ht="240">
+      <c r="A954">
+        <v>1244</v>
+      </c>
+      <c r="B954" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C954" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D954" t="s">
+        <v>15</v>
+      </c>
+      <c r="E954" t="s">
+        <v>16</v>
+      </c>
+      <c r="F954" s="16" t="s">
+        <v>1912</v>
+      </c>
+      <c r="G954">
+        <v>10006</v>
+      </c>
+      <c r="H954" t="s">
+        <v>404</v>
+      </c>
+      <c r="I954" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J954" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K954" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L954" t="s">
+        <v>22</v>
+      </c>
+      <c r="M954" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="955" spans="1:13" ht="315">
+      <c r="A955">
+        <v>1244</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C955" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D955" t="s">
+        <v>15</v>
+      </c>
+      <c r="E955" t="s">
+        <v>16</v>
+      </c>
+      <c r="F955" s="16" t="s">
+        <v>1913</v>
+      </c>
+      <c r="G955">
+        <v>10006</v>
+      </c>
+      <c r="H955" t="s">
+        <v>404</v>
+      </c>
+      <c r="I955" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J955" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K955" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L955" t="s">
+        <v>22</v>
+      </c>
+      <c r="M955" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="956" spans="1:13" ht="390">
+      <c r="A956">
+        <v>1244</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C956" t="s">
+        <v>1903</v>
+      </c>
+      <c r="D956" t="s">
+        <v>15</v>
+      </c>
+      <c r="E956" t="s">
+        <v>16</v>
+      </c>
+      <c r="F956" s="16" t="s">
+        <v>1914</v>
+      </c>
+      <c r="G956">
+        <v>10006</v>
+      </c>
+      <c r="H956" t="s">
+        <v>404</v>
+      </c>
+      <c r="I956" t="s">
+        <v>1904</v>
+      </c>
+      <c r="J956" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K956" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L956" t="s">
+        <v>22</v>
+      </c>
+      <c r="M956" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="957" spans="1:13" ht="210">
+      <c r="A957">
+        <v>1245</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C957" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D957" t="s">
+        <v>15</v>
+      </c>
+      <c r="E957" t="s">
+        <v>16</v>
+      </c>
+      <c r="F957" s="16" t="s">
+        <v>1915</v>
+      </c>
+      <c r="G957">
+        <v>10006</v>
+      </c>
+      <c r="H957" t="s">
+        <v>404</v>
+      </c>
+      <c r="I957" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J957" t="s">
+        <v>20</v>
+      </c>
+      <c r="K957" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L957" t="s">
+        <v>22</v>
+      </c>
+      <c r="M957" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="958" spans="1:13" ht="150">
+      <c r="A958">
+        <v>1245</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C958" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D958" t="s">
+        <v>15</v>
+      </c>
+      <c r="E958" t="s">
+        <v>16</v>
+      </c>
+      <c r="F958" s="16" t="s">
+        <v>1916</v>
+      </c>
+      <c r="G958">
+        <v>10006</v>
+      </c>
+      <c r="H958" t="s">
+        <v>404</v>
+      </c>
+      <c r="I958" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J958" t="s">
+        <v>43</v>
+      </c>
+      <c r="K958" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L958" t="s">
+        <v>22</v>
+      </c>
+      <c r="M958" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="959" spans="1:13" ht="210">
+      <c r="A959">
+        <v>1245</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C959" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D959" t="s">
+        <v>15</v>
+      </c>
+      <c r="E959" t="s">
+        <v>16</v>
+      </c>
+      <c r="F959" s="16" t="s">
+        <v>1917</v>
+      </c>
+      <c r="G959">
+        <v>10006</v>
+      </c>
+      <c r="H959" t="s">
+        <v>404</v>
+      </c>
+      <c r="I959" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J959" t="s">
+        <v>35</v>
+      </c>
+      <c r="K959" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L959" t="s">
+        <v>22</v>
+      </c>
+      <c r="M959" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="960" spans="1:13" ht="210">
+      <c r="A960">
+        <v>1245</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C960" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D960" t="s">
+        <v>15</v>
+      </c>
+      <c r="E960" t="s">
+        <v>16</v>
+      </c>
+      <c r="F960" s="16" t="s">
+        <v>1918</v>
+      </c>
+      <c r="G960">
+        <v>10006</v>
+      </c>
+      <c r="H960" t="s">
+        <v>404</v>
+      </c>
+      <c r="I960" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J960" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K960" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L960" t="s">
+        <v>22</v>
+      </c>
+      <c r="M960" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="961" spans="1:13" ht="285">
+      <c r="A961">
+        <v>1245</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C961" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D961" t="s">
+        <v>15</v>
+      </c>
+      <c r="E961" t="s">
+        <v>16</v>
+      </c>
+      <c r="F961" s="16" t="s">
+        <v>1919</v>
+      </c>
+      <c r="G961">
+        <v>10006</v>
+      </c>
+      <c r="H961" t="s">
+        <v>404</v>
+      </c>
+      <c r="I961" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J961" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K961" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L961" t="s">
+        <v>22</v>
+      </c>
+      <c r="M961" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="962" spans="1:13" ht="345">
+      <c r="A962">
+        <v>1245</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C962" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D962" t="s">
+        <v>15</v>
+      </c>
+      <c r="E962" t="s">
+        <v>16</v>
+      </c>
+      <c r="F962" s="16" t="s">
+        <v>1920</v>
+      </c>
+      <c r="G962">
+        <v>10006</v>
+      </c>
+      <c r="H962" t="s">
+        <v>404</v>
+      </c>
+      <c r="I962" t="s">
+        <v>1906</v>
+      </c>
+      <c r="J962" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K962" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L962" t="s">
+        <v>22</v>
+      </c>
+      <c r="M962" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="963" spans="1:13" ht="105">
+      <c r="A963">
+        <v>1246</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C963" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D963" t="s">
+        <v>15</v>
+      </c>
+      <c r="E963" t="s">
+        <v>16</v>
+      </c>
+      <c r="F963" s="16" t="s">
+        <v>1921</v>
+      </c>
+      <c r="G963">
+        <v>10006</v>
+      </c>
+      <c r="H963" t="s">
+        <v>404</v>
+      </c>
+      <c r="I963" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J963" t="s">
+        <v>20</v>
+      </c>
+      <c r="K963" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L963" t="s">
+        <v>22</v>
+      </c>
+      <c r="M963" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="964" spans="1:13" ht="90">
+      <c r="A964">
+        <v>1246</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C964" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D964" t="s">
+        <v>15</v>
+      </c>
+      <c r="E964" t="s">
+        <v>16</v>
+      </c>
+      <c r="F964" s="16" t="s">
+        <v>1922</v>
+      </c>
+      <c r="G964">
+        <v>10006</v>
+      </c>
+      <c r="H964" t="s">
+        <v>404</v>
+      </c>
+      <c r="I964" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J964" t="s">
+        <v>43</v>
+      </c>
+      <c r="K964" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L964" t="s">
+        <v>22</v>
+      </c>
+      <c r="M964" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="965" spans="1:13" ht="135">
+      <c r="A965">
+        <v>1246</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C965" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D965" t="s">
+        <v>15</v>
+      </c>
+      <c r="E965" t="s">
+        <v>16</v>
+      </c>
+      <c r="F965" s="16" t="s">
+        <v>1923</v>
+      </c>
+      <c r="G965">
+        <v>10006</v>
+      </c>
+      <c r="H965" t="s">
+        <v>404</v>
+      </c>
+      <c r="I965" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J965" t="s">
+        <v>35</v>
+      </c>
+      <c r="K965" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L965" t="s">
+        <v>22</v>
+      </c>
+      <c r="M965" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="966" spans="1:13" ht="135">
+      <c r="A966">
+        <v>1246</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C966" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D966" t="s">
+        <v>15</v>
+      </c>
+      <c r="E966" t="s">
+        <v>16</v>
+      </c>
+      <c r="F966" s="16" t="s">
+        <v>1924</v>
+      </c>
+      <c r="G966">
+        <v>10006</v>
+      </c>
+      <c r="H966" t="s">
+        <v>404</v>
+      </c>
+      <c r="I966" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J966" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K966" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L966" t="s">
+        <v>22</v>
+      </c>
+      <c r="M966" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="967" spans="1:13" ht="165">
+      <c r="A967">
+        <v>1246</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C967" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D967" t="s">
+        <v>15</v>
+      </c>
+      <c r="E967" t="s">
+        <v>16</v>
+      </c>
+      <c r="F967" s="16" t="s">
+        <v>1925</v>
+      </c>
+      <c r="G967">
+        <v>10006</v>
+      </c>
+      <c r="H967" t="s">
+        <v>404</v>
+      </c>
+      <c r="I967" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J967" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K967" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L967" t="s">
+        <v>22</v>
+      </c>
+      <c r="M967" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="968" spans="1:13" ht="195">
+      <c r="A968">
+        <v>1246</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C968" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D968" t="s">
+        <v>15</v>
+      </c>
+      <c r="E968" t="s">
+        <v>16</v>
+      </c>
+      <c r="F968" s="16" t="s">
+        <v>1926</v>
+      </c>
+      <c r="G968">
+        <v>10006</v>
+      </c>
+      <c r="H968" t="s">
+        <v>404</v>
+      </c>
+      <c r="I968" t="s">
+        <v>1908</v>
+      </c>
+      <c r="J968" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K968" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L968" t="s">
+        <v>22</v>
+      </c>
+      <c r="M968" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
added templates for summary
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF572292-B0BF-40E8-BD6B-35D826354CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0F1224-417D-482F-BE29-5936A8299380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18981" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19509" uniqueCount="2380">
   <si>
     <t>id</t>
   </si>
@@ -17012,6 +17012,216 @@
     <t>$authType ஐப் பூட்ட முயற்சி செய்யப்பட்டது
 $authType ஐ திறக்க முயற்சி செய்யப்பட்டது</t>
   </si>
+  <si>
+    <t>Success summary to customize and download my card</t>
+  </si>
+  <si>
+    <t>Success summary to order a physical card</t>
+  </si>
+  <si>
+    <t>Success summary to share my credential with a partner</t>
+  </si>
+  <si>
+    <t>Success summary to lock/unlock various authentication types</t>
+  </si>
+  <si>
+    <t>Success summary to self update demographic data</t>
+  </si>
+  <si>
+    <t>Success summary to generate or revoke VIDs</t>
+  </si>
+  <si>
+    <t>Success summary to get my UIN card</t>
+  </si>
+  <si>
+    <t>Success summary to verify my phone and email</t>
+  </si>
+  <si>
+    <t>cust-and-down-my-card-success-summary</t>
+  </si>
+  <si>
+    <t>order-a-physical-card-success-summary</t>
+  </si>
+  <si>
+    <t>share-cred-with-partner-success-summary</t>
+  </si>
+  <si>
+    <t>lock-unlock-auth-success-summary</t>
+  </si>
+  <si>
+    <t>update-demo-data-success-summary</t>
+  </si>
+  <si>
+    <t>gen-or-revoke-vid-success-summary</t>
+  </si>
+  <si>
+    <t>get-my-uin-card-success-summary</t>
+  </si>
+  <si>
+    <t>verify-my-phone-email-success-summary</t>
+  </si>
+  <si>
+    <t>Personalised card with the $attributes was generated successfully and sent to the registered email ID and/or phone number</t>
+  </si>
+  <si>
+    <t>Order for a physical card has been placed successfully with the partner</t>
+  </si>
+  <si>
+    <t>Your $attributes were successfully shared</t>
+  </si>
+  <si>
+    <t>Your $authType was locked successfully
+Your $authType was unlocked successfully</t>
+  </si>
+  <si>
+    <t>Your $attributes were updated successfully and sent to the registered email ID and/or phone number</t>
+  </si>
+  <si>
+    <t>$vidType VID *masked VID* was generated successfully
+$vidType VID *masked VID* was revoked successfully</t>
+  </si>
+  <si>
+    <t>UIN card was successfully sent to the registered email ID and/or phone number</t>
+  </si>
+  <si>
+    <t>Your phone number was successfully verified
+Your email ID was successfully verified</t>
+  </si>
+  <si>
+    <t>تم إنشاء بطاقة شخصية بسماattributes$ بنجاح وتم إرسالها إلى معرف البريد الإلكتروني المسجل و / أو رقم الهاتف</t>
+  </si>
+  <si>
+    <t>تم تقديم طلب للحصول على بطاقة فعلية بنجاح مع الشريك</t>
+  </si>
+  <si>
+    <t>تمت مشاركة سمات attributes$ الخاصة بك بنجاح</t>
+  </si>
+  <si>
+    <t>م قفل authType$ الخاص بك بنجاح
+تم إلغاء قفل  authType$ الخاص بك بنجاح</t>
+  </si>
+  <si>
+    <t>تم تحديث سمات attributes$ بنجاح وتم إرسالها إلى معرف البريد الإلكتروني المسجل و / أو رقم الهاتف</t>
+  </si>
+  <si>
+    <t>تم إنشاء  vidType VID$ * مقنع VID * بنجاح
+تم إبطال vidType VID$ * المقنع VID * بنجاح</t>
+  </si>
+  <si>
+    <t>تم إرسال بطاقة UIN بنجاح إلى معرف البريد الإلكتروني المسجل و / أو رقم الهاتف</t>
+  </si>
+  <si>
+    <t>تم التحقق من رقم هاتفك بنجاح
+تم التحقق من معرف البريد الإلكتروني الخاص بك بنجاح</t>
+  </si>
+  <si>
+    <t>La carte personnalisée avec les $attributes a été générée avec succès et envoyée à l'adresse e-mail et/ou au numéro de téléphone enregistrés</t>
+  </si>
+  <si>
+    <t>La commande d'une carte physique a été passée avec succès auprès du partenaire</t>
+  </si>
+  <si>
+    <t>Vos $attributes ont été partagés avec succès</t>
+  </si>
+  <si>
+    <t>Votre $authType a été verrouillé avec succès
+Votre $authType a été déverrouillé avec succès</t>
+  </si>
+  <si>
+    <t>Vos $attributes ont été mis à jour avec succès et envoyés à l'identifiant de messagerie et/ou au numéro de téléphone enregistrés</t>
+  </si>
+  <si>
+    <t>$vidType VID *VID masqué* a été généré avec succès
+$vidType VID *masked VID* a été révoqué avec succès</t>
+  </si>
+  <si>
+    <t>La carte UIN a été envoyée avec succès à l'adresse e-mail et/ou au numéro de téléphone enregistrés</t>
+  </si>
+  <si>
+    <t>Votre numéro de téléphone a été vérifié avec succès
+Votre identifiant de messagerie a été vérifié avec succès</t>
+  </si>
+  <si>
+    <t>$attributes वाला वैयक्तिकृत कार्ड सफलतापूर्वक जनरेट किया गया और पंजीकृत ईमेल आईडी और/या फ़ोन नंबर पर भेजा गया</t>
+  </si>
+  <si>
+    <t>फिजिकल कार्ड के लिए ऑर्डर पार्टनर को सफलतापूर्वक दे दिया गया है</t>
+  </si>
+  <si>
+    <t>आपकी $attributes सफलतापूर्वक साझा की ग</t>
+  </si>
+  <si>
+    <t>आपका $authType सफलतापूर्वक लॉक कर दिया गया था
+आपका $authType सफलतापूर्वक अनलॉक हो गया था</t>
+  </si>
+  <si>
+    <t>आपकी $attributes सफलतापूर्वक अपडेट की गईं और पंजीकृत ईमेल आईडी और/या फोन नंबर पर भेज दी गईं</t>
+  </si>
+  <si>
+    <t>$vidType VID *नकाबपोश VID* सफलतापूर्वक जनरेट किया गया
+$vidType VID *नकाबपोश VID* को सफलतापूर्वक निरस्त कर दिया गया</t>
+  </si>
+  <si>
+    <t>यूआईएन कार्ड सफलतापूर्वक पंजीकृत ईमेल आईडी और/या फोन नंबर पर भेजा गया था</t>
+  </si>
+  <si>
+    <t>आपका फ़ोन नंबर सफलतापूर्वक सत्यापित किया गया था
+आपकी ईमेल आईडी को सफलतापूर्व</t>
+  </si>
+  <si>
+    <t>$attributes ಜೊತೆಗೆ ವೈಯಕ್ತಿಕಗೊಳಿಸಿದ ಕಾರ್ಡ್ ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ರಚಿಸಲಾಗಿದೆ ಮತ್ತು ನೋಂದಾಯಿತ ಇಮೇಲ್ ID ಮತ್ತು/ಅಥವಾ ಫೋನ್ ಸಂಖ್ಯೆಗೆ ಕಳುಹಿಸಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ಪಾಲುದಾರರೊಂದಿಗೆ ಭೌತಿಕ ಕಾರ್ಡ್‌ಗಾಗಿ ಆರ್ಡರ್ ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಇರಿಸಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ನಿಮ್ಮ $attributes ಗುಣಲಕ್ಷಣಗಳನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಹಂಚಿಕೊಳ್ಳಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ನಿಮ್ಮ $authType ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಲಾಕ್ ಮಾಡಲಾಗಿದೆ
+ನಿಮ್ಮ $authType ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಅನ್‌ಲಾಕ್ ಮಾಡಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ನಿಮ್ಮ $attributes ಯಶಸ್ವಿಯಾಗಿ ನವೀಕರಿಸಲಾಗಿದೆ ಮತ್ತು ನೋಂದಾಯಿತ ಇಮೇಲ್ ID ಮತ್ತು/ಅಥವಾ ಫೋನ್ ಸಂಖ್ಯೆಗೆ ಕಳುಹಿಸಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>$vidType VID *ಮಾಸ್ಕ್ಡ್ VID* ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ರಚಿಸಲಾಗಿದೆ
+$vidType VID *ಮಾಸ್ಕ್ ಮಾಡಿದ VID* ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಹಿಂಪಡೆಯಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ನೋಂದಾಯಿತ ಇಮೇಲ್ ಐಡಿ ಮತ್ತು/ಅಥವಾ ಫೋನ್ ಸಂಖ್ಯೆಗೆ UIN ಕಾರ್ಡ್ ಅನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಕಳುಹಿಸಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>ನಿಮ್ಮ ಫೋನ್ ಸಂಖ್ಯೆಯನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಪರಿಶೀಲಿಸಲಾಗಿದೆ
+ನಿಮ್ಮ ಇಮೇಲ್ ಐಡಿಯನ್ನು ಯಶಸ್ವಿಯಾಗಿ ಪರಿಶೀಲಿಸಲಾಗಿದೆ</t>
+  </si>
+  <si>
+    <t>$attributes கொண்ட தனிப்பயனாக்கப்பட்ட அட்டை வெற்றிகரமாக உருவாக்கப்பட்டு, பதிவுசெய்யப்பட்ட மின்னஞ்சல் ஐடி மற்றும்/அல்லது தொலைபேசி எண்ணுக்கு அனுப்பப்பட்டது</t>
+  </si>
+  <si>
+    <t>பார்ட்னரிடம் உடல் அட்டைக்கான ஆர்டர் வெற்றிகரமாக வைக்கப்பட்டுள்ளது</t>
+  </si>
+  <si>
+    <t>உங்கள் $attributes புகள் வெற்றிகரமாகப் பகிரப்பட்டன</t>
+  </si>
+  <si>
+    <t>உங்கள் $authType வெற்றிகரமாக பூட்டப்பட்டது
+உங்கள் $authType வெற்றிகரமாக திறக்கப்பட்டது</t>
+  </si>
+  <si>
+    <t>உங்கள் $attributesக்கூறுகள் வெற்றிகரமாக புதுப்பிக்கப்பட்டு பதிவு செய்யப்பட்ட மின்னஞ்சல் ஐடி மற்றும்/அல்லது ஃபோன் எண்ணுக்கு அனுப்பப்பட்டது</t>
+  </si>
+  <si>
+    <t>$vidType VID *மாஸ்க் செய்யப்பட்ட VID* வெற்றிகரமாக உருவாக்கப்பட்டது
+$vidType VID *மாஸ்க் செய்யப்பட்ட VID* வெற்றிகரமாக திரும்பப் பெறப்பட்டது</t>
+  </si>
+  <si>
+    <t>UIN கார்டு பதிவு செய்யப்பட்ட மின்னஞ்சல் ஐடி மற்றும்/அல்லது தொலைபேசி எண்ணுக்கு வெற்றிகரமாக அனுப்பப்பட்டது</t>
+  </si>
+  <si>
+    <t>உங்கள் தொலைபேசி எண் வெற்றிகரமாகச் சரிபார்க்கப்பட்டது
+உங்கள் மின்னஞ்சல் ஐடி வெற்றிகரமாகச் சரிபார்க்கப்பட்டது</t>
+  </si>
 </sst>
 </file>
 
@@ -17099,7 +17309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -17193,6 +17403,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -17537,10 +17751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1641"/>
+  <dimension ref="A1:M1689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1591" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1597" sqref="F1597"/>
+    <sheetView tabSelected="1" topLeftCell="A1682" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1691" sqref="F1691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -84827,6 +85041,1974 @@
         <v>23</v>
       </c>
     </row>
+    <row r="1642" spans="1:13">
+      <c r="A1642">
+        <v>1360</v>
+      </c>
+      <c r="B1642" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1642" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1642" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1642" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1642" s="42" t="s">
+        <v>2332</v>
+      </c>
+      <c r="G1642" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1642" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1642" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1642" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1642" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1642" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1642" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:13">
+      <c r="A1643">
+        <v>1361</v>
+      </c>
+      <c r="B1643" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1643" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1643" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1643" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1643" s="42" t="s">
+        <v>2333</v>
+      </c>
+      <c r="G1643" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1643" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1643" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1643" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1643" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1643" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1643" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:13">
+      <c r="A1644">
+        <v>1362</v>
+      </c>
+      <c r="B1644" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1644" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1644" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1644" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1644" s="43" t="s">
+        <v>2334</v>
+      </c>
+      <c r="G1644" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1644" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1644" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1644" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1644" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1644" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1644" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:13">
+      <c r="A1645">
+        <v>1363</v>
+      </c>
+      <c r="B1645" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1645" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1645" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1645" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1645" s="43" t="s">
+        <v>2335</v>
+      </c>
+      <c r="G1645" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1645" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1645" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1645" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1645" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1645" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1645" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:13">
+      <c r="A1646">
+        <v>1364</v>
+      </c>
+      <c r="B1646" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1646" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1646" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1646" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1646" s="42" t="s">
+        <v>2336</v>
+      </c>
+      <c r="G1646" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1646" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1646" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1646" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1646" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1646" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1646" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:13">
+      <c r="A1647">
+        <v>1365</v>
+      </c>
+      <c r="B1647" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1647" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1647" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1647" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1647" s="42" t="s">
+        <v>2337</v>
+      </c>
+      <c r="G1647" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1647" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1647" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1647" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1647" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1647" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1647" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:13">
+      <c r="A1648">
+        <v>1366</v>
+      </c>
+      <c r="B1648" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1648" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1648" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1648" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1648" s="42" t="s">
+        <v>2338</v>
+      </c>
+      <c r="G1648" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1648" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1648" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1648" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1648" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1648" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1648" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:13">
+      <c r="A1649">
+        <v>1367</v>
+      </c>
+      <c r="B1649" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1649" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1649" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1649" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1649" s="43" t="s">
+        <v>2339</v>
+      </c>
+      <c r="G1649" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1649" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1649" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1649" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1649" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1649" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1649" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:13">
+      <c r="A1650" s="26">
+        <v>1360</v>
+      </c>
+      <c r="B1650" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1650" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1650" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1650" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1650" s="42" t="s">
+        <v>2340</v>
+      </c>
+      <c r="G1650" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1650" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1650" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1650" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1650" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1650" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1650" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:13">
+      <c r="A1651" s="26">
+        <v>1361</v>
+      </c>
+      <c r="B1651" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1651" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1651" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1651" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1651" s="42" t="s">
+        <v>2341</v>
+      </c>
+      <c r="G1651" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1651" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1651" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1651" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1651" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1651" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1651" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:13">
+      <c r="A1652" s="26">
+        <v>1362</v>
+      </c>
+      <c r="B1652" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1652" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1652" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1652" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1652" s="43" t="s">
+        <v>2342</v>
+      </c>
+      <c r="G1652" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1652" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1652" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1652" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1652" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1652" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1652" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:13">
+      <c r="A1653" s="26">
+        <v>1363</v>
+      </c>
+      <c r="B1653" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1653" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1653" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1653" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1653" s="43" t="s">
+        <v>2343</v>
+      </c>
+      <c r="G1653" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1653" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1653" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1653" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1653" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1653" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1653" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:13">
+      <c r="A1654" s="26">
+        <v>1364</v>
+      </c>
+      <c r="B1654" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1654" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1654" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1654" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1654" s="42" t="s">
+        <v>2344</v>
+      </c>
+      <c r="G1654" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1654" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1654" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1654" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1654" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1654" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1654" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:13">
+      <c r="A1655" s="26">
+        <v>1365</v>
+      </c>
+      <c r="B1655" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1655" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1655" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1655" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1655" s="42" t="s">
+        <v>2345</v>
+      </c>
+      <c r="G1655" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1655" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1655" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1655" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1655" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1655" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1655" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:13">
+      <c r="A1656" s="26">
+        <v>1366</v>
+      </c>
+      <c r="B1656" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1656" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1656" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1656" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1656" s="42" t="s">
+        <v>2346</v>
+      </c>
+      <c r="G1656" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1656" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1656" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1656" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1656" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1656" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1656" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:13">
+      <c r="A1657" s="26">
+        <v>1367</v>
+      </c>
+      <c r="B1657" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1657" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1657" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1657" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1657" s="43" t="s">
+        <v>2347</v>
+      </c>
+      <c r="G1657" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1657" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1657" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1657" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1657" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1657" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1657" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:13">
+      <c r="A1658" s="26">
+        <v>1360</v>
+      </c>
+      <c r="B1658" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1658" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1658" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1658" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1658" s="42" t="s">
+        <v>2348</v>
+      </c>
+      <c r="G1658" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1658" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1658" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1658" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1658" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1658" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1658" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:13">
+      <c r="A1659" s="26">
+        <v>1361</v>
+      </c>
+      <c r="B1659" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1659" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1659" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1659" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1659" s="42" t="s">
+        <v>2349</v>
+      </c>
+      <c r="G1659" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1659" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1659" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1659" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1659" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1659" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1659" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:13">
+      <c r="A1660" s="26">
+        <v>1362</v>
+      </c>
+      <c r="B1660" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1660" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1660" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1660" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1660" s="43" t="s">
+        <v>2350</v>
+      </c>
+      <c r="G1660" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1660" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1660" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1660" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1660" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1660" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1660" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:13">
+      <c r="A1661" s="26">
+        <v>1363</v>
+      </c>
+      <c r="B1661" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1661" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1661" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1661" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1661" s="43" t="s">
+        <v>2351</v>
+      </c>
+      <c r="G1661" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1661" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1661" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1661" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1661" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1661" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1661" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:13">
+      <c r="A1662" s="26">
+        <v>1364</v>
+      </c>
+      <c r="B1662" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1662" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1662" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1662" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1662" s="42" t="s">
+        <v>2352</v>
+      </c>
+      <c r="G1662" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1662" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1662" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1662" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1662" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1662" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1662" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:13">
+      <c r="A1663" s="26">
+        <v>1365</v>
+      </c>
+      <c r="B1663" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1663" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1663" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1663" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1663" s="42" t="s">
+        <v>2353</v>
+      </c>
+      <c r="G1663" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1663" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1663" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1663" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1663" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1663" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1663" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:13">
+      <c r="A1664" s="26">
+        <v>1366</v>
+      </c>
+      <c r="B1664" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1664" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1664" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1664" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1664" s="42" t="s">
+        <v>2354</v>
+      </c>
+      <c r="G1664" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1664" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1664" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1664" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1664" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1664" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1664" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:13">
+      <c r="A1665" s="26">
+        <v>1367</v>
+      </c>
+      <c r="B1665" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1665" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1665" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1665" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1665" s="43" t="s">
+        <v>2355</v>
+      </c>
+      <c r="G1665" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1665" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1665" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1665" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1665" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1665" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1665" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:13">
+      <c r="A1666" s="26">
+        <v>1360</v>
+      </c>
+      <c r="B1666" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1666" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1666" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1666" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1666" s="42" t="s">
+        <v>2356</v>
+      </c>
+      <c r="G1666" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1666" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1666" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1666" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1666" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1666" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1666" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:13">
+      <c r="A1667" s="26">
+        <v>1361</v>
+      </c>
+      <c r="B1667" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1667" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1667" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1667" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1667" s="42" t="s">
+        <v>2357</v>
+      </c>
+      <c r="G1667" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1667" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1667" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1667" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1667" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1667" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1667" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:13">
+      <c r="A1668" s="26">
+        <v>1362</v>
+      </c>
+      <c r="B1668" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1668" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1668" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1668" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1668" s="43" t="s">
+        <v>2358</v>
+      </c>
+      <c r="G1668" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1668" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1668" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1668" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1668" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1668" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1668" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:13">
+      <c r="A1669" s="26">
+        <v>1363</v>
+      </c>
+      <c r="B1669" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1669" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1669" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1669" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1669" s="43" t="s">
+        <v>2359</v>
+      </c>
+      <c r="G1669" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1669" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1669" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1669" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1669" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1669" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1669" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:13">
+      <c r="A1670" s="26">
+        <v>1364</v>
+      </c>
+      <c r="B1670" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1670" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1670" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1670" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1670" s="42" t="s">
+        <v>2360</v>
+      </c>
+      <c r="G1670" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1670" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1670" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1670" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1670" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1670" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1670" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:13">
+      <c r="A1671" s="26">
+        <v>1365</v>
+      </c>
+      <c r="B1671" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1671" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1671" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1671" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1671" s="42" t="s">
+        <v>2361</v>
+      </c>
+      <c r="G1671" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1671" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1671" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1671" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1671" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1671" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1671" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:13">
+      <c r="A1672" s="26">
+        <v>1366</v>
+      </c>
+      <c r="B1672" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1672" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1672" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1672" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1672" s="42" t="s">
+        <v>2362</v>
+      </c>
+      <c r="G1672" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1672" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1672" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1672" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1672" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1672" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1672" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:13">
+      <c r="A1673" s="26">
+        <v>1367</v>
+      </c>
+      <c r="B1673" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1673" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1673" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1673" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1673" s="43" t="s">
+        <v>2363</v>
+      </c>
+      <c r="G1673" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1673" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1673" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1673" s="26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="K1673" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1673" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1673" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:13">
+      <c r="A1674" s="26">
+        <v>1360</v>
+      </c>
+      <c r="B1674" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1674" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1674" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1674" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1674" s="42" t="s">
+        <v>2364</v>
+      </c>
+      <c r="G1674" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1674" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1674" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1674" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1674" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1674" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1674" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:13">
+      <c r="A1675" s="26">
+        <v>1361</v>
+      </c>
+      <c r="B1675" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1675" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1675" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1675" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1675" s="42" t="s">
+        <v>2365</v>
+      </c>
+      <c r="G1675" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1675" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1675" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1675" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1675" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1675" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1675" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:13">
+      <c r="A1676" s="26">
+        <v>1362</v>
+      </c>
+      <c r="B1676" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1676" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1676" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1676" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1676" s="43" t="s">
+        <v>2366</v>
+      </c>
+      <c r="G1676" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1676" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1676" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1676" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1676" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1676" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1676" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:13">
+      <c r="A1677" s="26">
+        <v>1363</v>
+      </c>
+      <c r="B1677" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1677" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1677" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1677" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1677" s="43" t="s">
+        <v>2367</v>
+      </c>
+      <c r="G1677" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1677" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1677" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1677" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1677" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1677" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1677" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:13">
+      <c r="A1678" s="26">
+        <v>1364</v>
+      </c>
+      <c r="B1678" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1678" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1678" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1678" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1678" s="42" t="s">
+        <v>2368</v>
+      </c>
+      <c r="G1678" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1678" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1678" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1678" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1678" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1678" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1678" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:13">
+      <c r="A1679" s="26">
+        <v>1365</v>
+      </c>
+      <c r="B1679" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1679" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1679" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1679" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1679" s="42" t="s">
+        <v>2369</v>
+      </c>
+      <c r="G1679" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1679" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1679" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1679" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1679" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1679" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1679" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:13">
+      <c r="A1680" s="26">
+        <v>1366</v>
+      </c>
+      <c r="B1680" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1680" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1680" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1680" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1680" s="42" t="s">
+        <v>2370</v>
+      </c>
+      <c r="G1680" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1680" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1680" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1680" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1680" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1680" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1680" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:13">
+      <c r="A1681" s="26">
+        <v>1367</v>
+      </c>
+      <c r="B1681" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1681" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1681" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1681" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1681" s="43" t="s">
+        <v>2371</v>
+      </c>
+      <c r="G1681" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1681" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1681" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1681" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="K1681" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1681" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1681" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:13">
+      <c r="A1682" s="26">
+        <v>1360</v>
+      </c>
+      <c r="B1682" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C1682" s="26" t="s">
+        <v>2316</v>
+      </c>
+      <c r="D1682" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1682" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1682" s="42" t="s">
+        <v>2372</v>
+      </c>
+      <c r="G1682" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1682" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1682" s="26" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J1682" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1682" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1682" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1682" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:13">
+      <c r="A1683" s="26">
+        <v>1361</v>
+      </c>
+      <c r="B1683" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1683" s="26" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D1683" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1683" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1683" s="42" t="s">
+        <v>2373</v>
+      </c>
+      <c r="G1683" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1683" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1683" s="26" t="s">
+        <v>2325</v>
+      </c>
+      <c r="J1683" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1683" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1683" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1683" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:13">
+      <c r="A1684" s="26">
+        <v>1362</v>
+      </c>
+      <c r="B1684" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1684" s="26" t="s">
+        <v>2318</v>
+      </c>
+      <c r="D1684" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1684" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1684" s="43" t="s">
+        <v>2374</v>
+      </c>
+      <c r="G1684" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1684" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1684" s="26" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J1684" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1684" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1684" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1684" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:13">
+      <c r="A1685" s="26">
+        <v>1363</v>
+      </c>
+      <c r="B1685" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1685" s="26" t="s">
+        <v>2319</v>
+      </c>
+      <c r="D1685" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1685" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1685" s="43" t="s">
+        <v>2375</v>
+      </c>
+      <c r="G1685" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1685" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1685" s="26" t="s">
+        <v>2327</v>
+      </c>
+      <c r="J1685" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1685" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1685" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1685" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:13">
+      <c r="A1686" s="26">
+        <v>1364</v>
+      </c>
+      <c r="B1686" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1686" s="26" t="s">
+        <v>2320</v>
+      </c>
+      <c r="D1686" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1686" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1686" s="42" t="s">
+        <v>2376</v>
+      </c>
+      <c r="G1686" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1686" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1686" s="26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="J1686" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1686" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1686" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1686" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:13">
+      <c r="A1687" s="26">
+        <v>1365</v>
+      </c>
+      <c r="B1687" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C1687" s="26" t="s">
+        <v>2321</v>
+      </c>
+      <c r="D1687" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1687" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1687" s="42" t="s">
+        <v>2377</v>
+      </c>
+      <c r="G1687" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1687" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1687" s="26" t="s">
+        <v>2329</v>
+      </c>
+      <c r="J1687" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1687" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1687" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1687" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:13">
+      <c r="A1688" s="26">
+        <v>1366</v>
+      </c>
+      <c r="B1688" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1688" s="26" t="s">
+        <v>2322</v>
+      </c>
+      <c r="D1688" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1688" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1688" s="42" t="s">
+        <v>2378</v>
+      </c>
+      <c r="G1688" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1688" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1688" s="26" t="s">
+        <v>2330</v>
+      </c>
+      <c r="J1688" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1688" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1688" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1688" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:13">
+      <c r="A1689" s="26">
+        <v>1367</v>
+      </c>
+      <c r="B1689" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C1689" s="26" t="s">
+        <v>2323</v>
+      </c>
+      <c r="D1689" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1689" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1689" s="43" t="s">
+        <v>2379</v>
+      </c>
+      <c r="G1689" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1689" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1689" s="26" t="s">
+        <v>2331</v>
+      </c>
+      <c r="J1689" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="K1689" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1689" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1689" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
give new ids to duplicates
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0F1224-417D-482F-BE29-5936A8299380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E6B413-3435-4CF3-895B-6B3C5F55A775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17753,8 +17753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1682" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1691" sqref="F1691"/>
+    <sheetView tabSelected="1" topLeftCell="A1184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1197" sqref="D1197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -58188,7 +58188,7 @@
     </row>
     <row r="987" spans="1:13" ht="60">
       <c r="A987">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B987" t="s">
         <v>1938</v>
@@ -58229,7 +58229,7 @@
     </row>
     <row r="988" spans="1:13" ht="45">
       <c r="A988">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B988" t="s">
         <v>1938</v>
@@ -58270,7 +58270,7 @@
     </row>
     <row r="989" spans="1:13" ht="60">
       <c r="A989">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B989" t="s">
         <v>1938</v>
@@ -58311,7 +58311,7 @@
     </row>
     <row r="990" spans="1:13" ht="60">
       <c r="A990">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B990" t="s">
         <v>1938</v>
@@ -58352,7 +58352,7 @@
     </row>
     <row r="991" spans="1:13" ht="60">
       <c r="A991">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B991" t="s">
         <v>1938</v>
@@ -58393,7 +58393,7 @@
     </row>
     <row r="992" spans="1:13" ht="60">
       <c r="A992">
-        <v>1250</v>
+        <v>1368</v>
       </c>
       <c r="B992" t="s">
         <v>1938</v>
@@ -58926,7 +58926,7 @@
     </row>
     <row r="1005" spans="1:13" ht="30">
       <c r="A1005">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1005" t="s">
         <v>1963</v>
@@ -58967,7 +58967,7 @@
     </row>
     <row r="1006" spans="1:13" ht="30">
       <c r="A1006">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1006" t="s">
         <v>1963</v>
@@ -59008,7 +59008,7 @@
     </row>
     <row r="1007" spans="1:13" ht="30">
       <c r="A1007">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1007" t="s">
         <v>1963</v>
@@ -59049,7 +59049,7 @@
     </row>
     <row r="1008" spans="1:13" ht="30">
       <c r="A1008">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1008" t="s">
         <v>1963</v>
@@ -59090,7 +59090,7 @@
     </row>
     <row r="1009" spans="1:13" ht="30">
       <c r="A1009">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1009" t="s">
         <v>1963</v>
@@ -59131,7 +59131,7 @@
     </row>
     <row r="1010" spans="1:13" ht="30">
       <c r="A1010">
-        <v>1253</v>
+        <v>1369</v>
       </c>
       <c r="B1010" t="s">
         <v>1963</v>
@@ -60648,7 +60648,7 @@
     </row>
     <row r="1047" spans="1:13" ht="30">
       <c r="A1047">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1047" t="s">
         <v>1985</v>
@@ -60689,7 +60689,7 @@
     </row>
     <row r="1048" spans="1:13" ht="30">
       <c r="A1048">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1048" t="s">
         <v>1985</v>
@@ -60730,7 +60730,7 @@
     </row>
     <row r="1049" spans="1:13" ht="30">
       <c r="A1049">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1049" t="s">
         <v>1985</v>
@@ -60771,7 +60771,7 @@
     </row>
     <row r="1050" spans="1:13" ht="30">
       <c r="A1050">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1050" t="s">
         <v>1985</v>
@@ -60812,7 +60812,7 @@
     </row>
     <row r="1051" spans="1:13" ht="30">
       <c r="A1051">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1051" t="s">
         <v>1985</v>
@@ -60853,7 +60853,7 @@
     </row>
     <row r="1052" spans="1:13" ht="30">
       <c r="A1052">
-        <v>1260</v>
+        <v>1370</v>
       </c>
       <c r="B1052" t="s">
         <v>1985</v>
@@ -61386,7 +61386,7 @@
     </row>
     <row r="1065" spans="1:13" ht="60">
       <c r="A1065">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1065" t="s">
         <v>1988</v>
@@ -61427,7 +61427,7 @@
     </row>
     <row r="1066" spans="1:13" ht="60">
       <c r="A1066">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1066" t="s">
         <v>1988</v>
@@ -61468,7 +61468,7 @@
     </row>
     <row r="1067" spans="1:13" ht="60">
       <c r="A1067">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1067" t="s">
         <v>1988</v>
@@ -61509,7 +61509,7 @@
     </row>
     <row r="1068" spans="1:13" ht="60">
       <c r="A1068">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1068" t="s">
         <v>1988</v>
@@ -61550,7 +61550,7 @@
     </row>
     <row r="1069" spans="1:13" ht="75">
       <c r="A1069">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1069" t="s">
         <v>1988</v>
@@ -61591,7 +61591,7 @@
     </row>
     <row r="1070" spans="1:13" ht="75">
       <c r="A1070">
-        <v>1263</v>
+        <v>1371</v>
       </c>
       <c r="B1070" t="s">
         <v>1988</v>
@@ -61632,7 +61632,7 @@
     </row>
     <row r="1071" spans="1:13" ht="90">
       <c r="A1071">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1071" t="s">
         <v>1989</v>
@@ -61673,7 +61673,7 @@
     </row>
     <row r="1072" spans="1:13" ht="90">
       <c r="A1072">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1072" t="s">
         <v>1989</v>
@@ -61714,7 +61714,7 @@
     </row>
     <row r="1073" spans="1:13" ht="90">
       <c r="A1073">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1073" t="s">
         <v>1989</v>
@@ -61755,7 +61755,7 @@
     </row>
     <row r="1074" spans="1:13" ht="90">
       <c r="A1074">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1074" t="s">
         <v>1989</v>
@@ -61796,7 +61796,7 @@
     </row>
     <row r="1075" spans="1:13" ht="90">
       <c r="A1075">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1075" t="s">
         <v>1989</v>
@@ -61837,7 +61837,7 @@
     </row>
     <row r="1076" spans="1:13" ht="120">
       <c r="A1076">
-        <v>1264</v>
+        <v>1372</v>
       </c>
       <c r="B1076" t="s">
         <v>1989</v>
@@ -61878,7 +61878,7 @@
     </row>
     <row r="1077" spans="1:13" ht="30">
       <c r="A1077">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1077" t="s">
         <v>1993</v>
@@ -61919,7 +61919,7 @@
     </row>
     <row r="1078" spans="1:13" ht="30">
       <c r="A1078">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1078" t="s">
         <v>1993</v>
@@ -61960,7 +61960,7 @@
     </row>
     <row r="1079" spans="1:13" ht="30">
       <c r="A1079">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1079" t="s">
         <v>1993</v>
@@ -62001,7 +62001,7 @@
     </row>
     <row r="1080" spans="1:13" ht="30">
       <c r="A1080">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1080" t="s">
         <v>1993</v>
@@ -62042,7 +62042,7 @@
     </row>
     <row r="1081" spans="1:13" ht="30">
       <c r="A1081">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1081" t="s">
         <v>1993</v>
@@ -62083,7 +62083,7 @@
     </row>
     <row r="1082" spans="1:13" ht="30">
       <c r="A1082">
-        <v>1265</v>
+        <v>1373</v>
       </c>
       <c r="B1082" t="s">
         <v>1993</v>
@@ -62124,7 +62124,7 @@
     </row>
     <row r="1083" spans="1:13" ht="30">
       <c r="A1083">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1083" t="s">
         <v>1994</v>
@@ -62165,7 +62165,7 @@
     </row>
     <row r="1084" spans="1:13" ht="30">
       <c r="A1084">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1084" t="s">
         <v>1994</v>
@@ -62206,7 +62206,7 @@
     </row>
     <row r="1085" spans="1:13" ht="30">
       <c r="A1085">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1085" t="s">
         <v>1994</v>
@@ -62247,7 +62247,7 @@
     </row>
     <row r="1086" spans="1:13" ht="30">
       <c r="A1086">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1086" t="s">
         <v>1994</v>
@@ -62288,7 +62288,7 @@
     </row>
     <row r="1087" spans="1:13" ht="30">
       <c r="A1087">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1087" t="s">
         <v>1994</v>
@@ -62329,7 +62329,7 @@
     </row>
     <row r="1088" spans="1:13" ht="30">
       <c r="A1088">
-        <v>1266</v>
+        <v>1374</v>
       </c>
       <c r="B1088" t="s">
         <v>1994</v>
@@ -62370,7 +62370,7 @@
     </row>
     <row r="1089" spans="1:13" ht="30">
       <c r="A1089">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1089" t="s">
         <v>1995</v>
@@ -62411,7 +62411,7 @@
     </row>
     <row r="1090" spans="1:13" ht="30">
       <c r="A1090">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1090" t="s">
         <v>1995</v>
@@ -62452,7 +62452,7 @@
     </row>
     <row r="1091" spans="1:13" ht="30">
       <c r="A1091">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1091" t="s">
         <v>1995</v>
@@ -62493,7 +62493,7 @@
     </row>
     <row r="1092" spans="1:13" ht="30">
       <c r="A1092">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1092" t="s">
         <v>1995</v>
@@ -62534,7 +62534,7 @@
     </row>
     <row r="1093" spans="1:13" ht="30">
       <c r="A1093">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1093" t="s">
         <v>1995</v>
@@ -62575,7 +62575,7 @@
     </row>
     <row r="1094" spans="1:13" ht="30">
       <c r="A1094">
-        <v>1267</v>
+        <v>1375</v>
       </c>
       <c r="B1094" t="s">
         <v>1995</v>
@@ -62616,7 +62616,7 @@
     </row>
     <row r="1095" spans="1:13" ht="60">
       <c r="A1095">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1095" t="s">
         <v>1996</v>
@@ -62657,7 +62657,7 @@
     </row>
     <row r="1096" spans="1:13" ht="60">
       <c r="A1096">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1096" t="s">
         <v>1997</v>
@@ -62739,7 +62739,7 @@
     </row>
     <row r="1098" spans="1:13" ht="45">
       <c r="A1098">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1098" t="s">
         <v>1996</v>
@@ -62780,7 +62780,7 @@
     </row>
     <row r="1099" spans="1:13" ht="45">
       <c r="A1099">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1099" t="s">
         <v>1997</v>
@@ -62862,7 +62862,7 @@
     </row>
     <row r="1101" spans="1:13" ht="60">
       <c r="A1101">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1101" t="s">
         <v>1996</v>
@@ -62903,7 +62903,7 @@
     </row>
     <row r="1102" spans="1:13" ht="60">
       <c r="A1102">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1102" t="s">
         <v>1997</v>
@@ -62985,7 +62985,7 @@
     </row>
     <row r="1104" spans="1:13" ht="60">
       <c r="A1104">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1104" t="s">
         <v>1996</v>
@@ -63026,7 +63026,7 @@
     </row>
     <row r="1105" spans="1:13" ht="60">
       <c r="A1105">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1105" t="s">
         <v>1997</v>
@@ -63108,7 +63108,7 @@
     </row>
     <row r="1107" spans="1:13" ht="60">
       <c r="A1107">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1107" t="s">
         <v>1996</v>
@@ -63149,7 +63149,7 @@
     </row>
     <row r="1108" spans="1:13" ht="60">
       <c r="A1108">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1108" t="s">
         <v>1997</v>
@@ -63231,7 +63231,7 @@
     </row>
     <row r="1110" spans="1:13" ht="60">
       <c r="A1110">
-        <v>1268</v>
+        <v>1376</v>
       </c>
       <c r="B1110" t="s">
         <v>1996</v>
@@ -63272,7 +63272,7 @@
     </row>
     <row r="1111" spans="1:13" ht="75">
       <c r="A1111">
-        <v>1269</v>
+        <v>1377</v>
       </c>
       <c r="B1111" t="s">
         <v>1997</v>
@@ -63600,7 +63600,7 @@
     </row>
     <row r="1119" spans="1:13" ht="30">
       <c r="A1119">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1119" t="s">
         <v>2012</v>
@@ -63641,7 +63641,7 @@
     </row>
     <row r="1120" spans="1:13" ht="30">
       <c r="A1120">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1120" t="s">
         <v>2012</v>
@@ -63682,7 +63682,7 @@
     </row>
     <row r="1121" spans="1:13" ht="30">
       <c r="A1121">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1121" t="s">
         <v>2012</v>
@@ -63723,7 +63723,7 @@
     </row>
     <row r="1122" spans="1:13" ht="30">
       <c r="A1122">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1122" t="s">
         <v>2012</v>
@@ -63764,7 +63764,7 @@
     </row>
     <row r="1123" spans="1:13" ht="30">
       <c r="A1123">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1123" t="s">
         <v>2012</v>
@@ -63805,7 +63805,7 @@
     </row>
     <row r="1124" spans="1:13" ht="30">
       <c r="A1124">
-        <v>1272</v>
+        <v>1378</v>
       </c>
       <c r="B1124" t="s">
         <v>2012</v>
@@ -63846,7 +63846,7 @@
     </row>
     <row r="1125" spans="1:13" ht="30">
       <c r="A1125">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1125" t="s">
         <v>2013</v>
@@ -63887,7 +63887,7 @@
     </row>
     <row r="1126" spans="1:13" ht="30">
       <c r="A1126">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1126" t="s">
         <v>2013</v>
@@ -63928,7 +63928,7 @@
     </row>
     <row r="1127" spans="1:13" ht="30">
       <c r="A1127">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1127" t="s">
         <v>2013</v>
@@ -63969,7 +63969,7 @@
     </row>
     <row r="1128" spans="1:13" ht="30">
       <c r="A1128">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1128" t="s">
         <v>2013</v>
@@ -64010,7 +64010,7 @@
     </row>
     <row r="1129" spans="1:13" ht="30">
       <c r="A1129">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1129" t="s">
         <v>2013</v>
@@ -64051,7 +64051,7 @@
     </row>
     <row r="1130" spans="1:13" ht="30">
       <c r="A1130">
-        <v>1273</v>
+        <v>1379</v>
       </c>
       <c r="B1130" t="s">
         <v>2013</v>
@@ -64092,7 +64092,7 @@
     </row>
     <row r="1131" spans="1:13" ht="60">
       <c r="A1131">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1131" t="s">
         <v>2014</v>
@@ -64133,7 +64133,7 @@
     </row>
     <row r="1132" spans="1:13" ht="105">
       <c r="A1132">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1132" t="s">
         <v>2015</v>
@@ -64174,7 +64174,7 @@
     </row>
     <row r="1133" spans="1:13" ht="90">
       <c r="A1133">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1133" t="s">
         <v>2016</v>
@@ -64215,7 +64215,7 @@
     </row>
     <row r="1134" spans="1:13" ht="45">
       <c r="A1134">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1134" t="s">
         <v>2014</v>
@@ -64256,7 +64256,7 @@
     </row>
     <row r="1135" spans="1:13" ht="75">
       <c r="A1135">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1135" t="s">
         <v>2015</v>
@@ -64297,7 +64297,7 @@
     </row>
     <row r="1136" spans="1:13" ht="90">
       <c r="A1136">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1136" t="s">
         <v>2016</v>
@@ -64338,7 +64338,7 @@
     </row>
     <row r="1137" spans="1:13" ht="60">
       <c r="A1137">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1137" t="s">
         <v>2014</v>
@@ -64379,7 +64379,7 @@
     </row>
     <row r="1138" spans="1:13" ht="105">
       <c r="A1138">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1138" t="s">
         <v>2015</v>
@@ -64420,7 +64420,7 @@
     </row>
     <row r="1139" spans="1:13" ht="90">
       <c r="A1139">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1139" t="s">
         <v>2016</v>
@@ -64461,7 +64461,7 @@
     </row>
     <row r="1140" spans="1:13" ht="60">
       <c r="A1140">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1140" t="s">
         <v>2014</v>
@@ -64502,7 +64502,7 @@
     </row>
     <row r="1141" spans="1:13" ht="105">
       <c r="A1141">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1141" t="s">
         <v>2015</v>
@@ -64543,7 +64543,7 @@
     </row>
     <row r="1142" spans="1:13" ht="90">
       <c r="A1142">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1142" t="s">
         <v>2016</v>
@@ -64584,7 +64584,7 @@
     </row>
     <row r="1143" spans="1:13" ht="60">
       <c r="A1143">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1143" t="s">
         <v>2014</v>
@@ -64625,7 +64625,7 @@
     </row>
     <row r="1144" spans="1:13" ht="120">
       <c r="A1144">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1144" t="s">
         <v>2015</v>
@@ -64666,7 +64666,7 @@
     </row>
     <row r="1145" spans="1:13" ht="90">
       <c r="A1145">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1145" t="s">
         <v>2016</v>
@@ -64707,7 +64707,7 @@
     </row>
     <row r="1146" spans="1:13" ht="60">
       <c r="A1146">
-        <v>1274</v>
+        <v>1380</v>
       </c>
       <c r="B1146" t="s">
         <v>2014</v>
@@ -64748,7 +64748,7 @@
     </row>
     <row r="1147" spans="1:13" ht="150">
       <c r="A1147">
-        <v>1275</v>
+        <v>1381</v>
       </c>
       <c r="B1147" t="s">
         <v>2015</v>
@@ -64789,7 +64789,7 @@
     </row>
     <row r="1148" spans="1:13" ht="120">
       <c r="A1148">
-        <v>1276</v>
+        <v>1382</v>
       </c>
       <c r="B1148" t="s">
         <v>2016</v>
@@ -64830,7 +64830,7 @@
     </row>
     <row r="1149" spans="1:13" ht="30">
       <c r="A1149">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1149" t="s">
         <v>2035</v>
@@ -64871,7 +64871,7 @@
     </row>
     <row r="1150" spans="1:13" ht="30">
       <c r="A1150">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1150" t="s">
         <v>2035</v>
@@ -64912,7 +64912,7 @@
     </row>
     <row r="1151" spans="1:13" ht="30">
       <c r="A1151">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1151" t="s">
         <v>2035</v>
@@ -64953,7 +64953,7 @@
     </row>
     <row r="1152" spans="1:13" ht="30">
       <c r="A1152">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1152" t="s">
         <v>2035</v>
@@ -64994,7 +64994,7 @@
     </row>
     <row r="1153" spans="1:13" ht="30">
       <c r="A1153">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1153" t="s">
         <v>2035</v>
@@ -65035,7 +65035,7 @@
     </row>
     <row r="1154" spans="1:13" ht="30">
       <c r="A1154">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="B1154" t="s">
         <v>2035</v>
@@ -65076,7 +65076,7 @@
     </row>
     <row r="1155" spans="1:13" ht="30">
       <c r="A1155">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1155" t="s">
         <v>2036</v>
@@ -65117,7 +65117,7 @@
     </row>
     <row r="1156" spans="1:13" ht="30">
       <c r="A1156">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1156" t="s">
         <v>2036</v>
@@ -65158,7 +65158,7 @@
     </row>
     <row r="1157" spans="1:13" ht="30">
       <c r="A1157">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1157" t="s">
         <v>2036</v>
@@ -65199,7 +65199,7 @@
     </row>
     <row r="1158" spans="1:13" ht="30">
       <c r="A1158">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1158" t="s">
         <v>2036</v>
@@ -65240,7 +65240,7 @@
     </row>
     <row r="1159" spans="1:13" ht="30">
       <c r="A1159">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1159" t="s">
         <v>2036</v>
@@ -65281,7 +65281,7 @@
     </row>
     <row r="1160" spans="1:13" ht="30">
       <c r="A1160">
-        <v>1278</v>
+        <v>1384</v>
       </c>
       <c r="B1160" t="s">
         <v>2036</v>
@@ -65322,7 +65322,7 @@
     </row>
     <row r="1161" spans="1:13" ht="30">
       <c r="A1161">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1161" t="s">
         <v>2037</v>
@@ -65363,7 +65363,7 @@
     </row>
     <row r="1162" spans="1:13" ht="30">
       <c r="A1162">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1162" t="s">
         <v>2037</v>
@@ -65404,7 +65404,7 @@
     </row>
     <row r="1163" spans="1:13" ht="30">
       <c r="A1163">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1163" t="s">
         <v>2037</v>
@@ -65445,7 +65445,7 @@
     </row>
     <row r="1164" spans="1:13" ht="30">
       <c r="A1164">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1164" t="s">
         <v>2037</v>
@@ -65486,7 +65486,7 @@
     </row>
     <row r="1165" spans="1:13" ht="30">
       <c r="A1165">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1165" t="s">
         <v>2037</v>
@@ -65527,7 +65527,7 @@
     </row>
     <row r="1166" spans="1:13" ht="30">
       <c r="A1166">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="B1166" t="s">
         <v>2037</v>
@@ -65568,7 +65568,7 @@
     </row>
     <row r="1167" spans="1:13" ht="60">
       <c r="A1167">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1167" t="s">
         <v>2038</v>
@@ -65609,7 +65609,7 @@
     </row>
     <row r="1168" spans="1:13" ht="60">
       <c r="A1168">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1168" t="s">
         <v>2039</v>
@@ -65691,7 +65691,7 @@
     </row>
     <row r="1170" spans="1:13" ht="45">
       <c r="A1170">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1170" t="s">
         <v>2038</v>
@@ -65732,7 +65732,7 @@
     </row>
     <row r="1171" spans="1:13" ht="45">
       <c r="A1171">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1171" t="s">
         <v>2039</v>
@@ -65814,7 +65814,7 @@
     </row>
     <row r="1173" spans="1:13" ht="60">
       <c r="A1173">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1173" t="s">
         <v>2038</v>
@@ -65855,7 +65855,7 @@
     </row>
     <row r="1174" spans="1:13" ht="60">
       <c r="A1174">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1174" t="s">
         <v>2039</v>
@@ -65937,7 +65937,7 @@
     </row>
     <row r="1176" spans="1:13" ht="60">
       <c r="A1176">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1176" t="s">
         <v>2038</v>
@@ -65978,7 +65978,7 @@
     </row>
     <row r="1177" spans="1:13" ht="60">
       <c r="A1177">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1177" t="s">
         <v>2039</v>
@@ -66060,7 +66060,7 @@
     </row>
     <row r="1179" spans="1:13" ht="60">
       <c r="A1179">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1179" t="s">
         <v>2038</v>
@@ -66101,7 +66101,7 @@
     </row>
     <row r="1180" spans="1:13" ht="60">
       <c r="A1180">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1180" t="s">
         <v>2039</v>
@@ -66183,7 +66183,7 @@
     </row>
     <row r="1182" spans="1:13" ht="60">
       <c r="A1182">
-        <v>1280</v>
+        <v>1386</v>
       </c>
       <c r="B1182" t="s">
         <v>2038</v>
@@ -66224,7 +66224,7 @@
     </row>
     <row r="1183" spans="1:13" ht="75">
       <c r="A1183">
-        <v>1281</v>
+        <v>1387</v>
       </c>
       <c r="B1183" t="s">
         <v>2039</v>
@@ -66306,7 +66306,7 @@
     </row>
     <row r="1185" spans="1:13" ht="30">
       <c r="A1185">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1185" t="s">
         <v>2047</v>
@@ -66347,7 +66347,7 @@
     </row>
     <row r="1186" spans="1:13" ht="30">
       <c r="A1186">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1186" t="s">
         <v>2047</v>
@@ -66388,7 +66388,7 @@
     </row>
     <row r="1187" spans="1:13" ht="30">
       <c r="A1187">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1187" t="s">
         <v>2047</v>
@@ -66429,7 +66429,7 @@
     </row>
     <row r="1188" spans="1:13" ht="30">
       <c r="A1188">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1188" t="s">
         <v>2047</v>
@@ -66470,7 +66470,7 @@
     </row>
     <row r="1189" spans="1:13" ht="30">
       <c r="A1189">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1189" t="s">
         <v>2047</v>
@@ -66511,7 +66511,7 @@
     </row>
     <row r="1190" spans="1:13" ht="30">
       <c r="A1190">
-        <v>1283</v>
+        <v>1388</v>
       </c>
       <c r="B1190" t="s">
         <v>2047</v>
@@ -66552,7 +66552,7 @@
     </row>
     <row r="1191" spans="1:13" ht="30">
       <c r="A1191">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1191" t="s">
         <v>2048</v>
@@ -66593,7 +66593,7 @@
     </row>
     <row r="1192" spans="1:13" ht="30">
       <c r="A1192">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1192" t="s">
         <v>2048</v>
@@ -66634,7 +66634,7 @@
     </row>
     <row r="1193" spans="1:13" ht="30">
       <c r="A1193">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1193" t="s">
         <v>2048</v>
@@ -66675,7 +66675,7 @@
     </row>
     <row r="1194" spans="1:13" ht="30">
       <c r="A1194">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1194" t="s">
         <v>2048</v>
@@ -66716,7 +66716,7 @@
     </row>
     <row r="1195" spans="1:13" ht="30">
       <c r="A1195">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1195" t="s">
         <v>2048</v>
@@ -66757,7 +66757,7 @@
     </row>
     <row r="1196" spans="1:13" ht="30">
       <c r="A1196">
-        <v>1284</v>
+        <v>1389</v>
       </c>
       <c r="B1196" t="s">
         <v>2048</v>

</xml_diff>

<commit_message>
added template for list of supporting docs
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D97CF-F8D8-4FF6-AED4-27C7080C4890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C605D0-0944-40DE-A766-5D7922C7D497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19509" uniqueCount="2380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19520" uniqueCount="2383">
   <si>
     <t>id</t>
   </si>
@@ -17238,6 +17238,374 @@
 &lt;/div&gt;
 &lt;/body&gt;
 &lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>List of supporting documents</t>
+  </si>
+  <si>
+    <t>supporting-docs-list</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;
+&lt;head&gt;
+&lt;/head&gt;
+&lt;body lang=EN-US style='word-wrap:break-word'&gt;
+&lt;div class=WordSection1&gt;
+&lt;p class=MsoNormal align=center style='text-align:center'&gt;&lt;b&gt;&lt;span
+style='font-size:16.0pt;line-height:107%;font-family:"Arial",sans-serif;
+color:#1D1C1D;background:yellow'&gt;Supporting documents&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;table class=MsoTableGrid border=1 cellspacing=0 cellpadding=0
+ style='border-collapse:collapse;border:none'&gt;
+ &lt;tr&gt;
+  &lt;td width=623 colspan=2 valign=top style='width:467.5pt;border:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:aqua'&gt;POI (&lt;/span&gt;&lt;/b&gt;&lt;b&gt;&lt;span style='font-size:
+  14.0pt;background:aqua'&gt;Proof of Identity)&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr style='height:35.85pt'&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt;height:35.85pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;The POI documents specification:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt;height:35.85pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;1. It should contain the Full Name and a clear Photo &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;2. It should be valid for at least the next 6 months&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;Acceptable document:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='font-size:16.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;1. Passport &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;2. PAN Card/ e-PAN &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;3. Ration / PDS Photo Card&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;4. Voter ID/ e-Voter ID &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;5. Driving License &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;6. Service photo identity card issued by Central Govt./ State Govt./ UT
+  Govt./ PSU/ Banks &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;7. Pensioner Photo Card/Freedom Fighter Photo Card &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;8. Disability ID Card/ handicapped medical certificate issued by the
+  respective Central/ State/ UT Governments&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;9. Bank Pass Book having name and Photograph Cross Stamped by bank
+  official&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;10. Valid Visa along with Foreign Passport&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+&lt;/table&gt;
+&lt;p class=MsoNormal&gt;&lt;span style='font-size:16.0pt;line-height:107%;font-family:
+"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;table class=MsoTableGrid border=1 cellspacing=0 cellpadding=0
+ style='border-collapse:collapse;border:none'&gt;
+ &lt;tr&gt;
+  &lt;td width=623 colspan=2 valign=top style='width:467.5pt;border:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:aqua'&gt;POA (Proof of Address)&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr style='height:35.3pt'&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt;height:35.3pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;The POA documents specification:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt;height:35.3pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;1. It should contain Full Name and full address &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;2. It should be valid for at least the next 6 months&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;Acceptable document:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='font-size:16.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;1. Passport/ Passport of Spouse/ Passport of Parents (in case of Minor)&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;2. Bank Statement (with Bank stamp &amp;amp; signature of bank official)/ Passbook/ Post
+  Office Account Statement/ Passbook&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;3. Ration Card&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;4. Voter ID/ e-Voter ID&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; 
+  &lt;/span&gt;5. Driving License&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;6. Service
+  photo identity card issued by PSU/ Banks/ State/ Central Governments&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;7. Pensioner
+  Card/ Freedom Fighter Card&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;8. Kissan
+  Passbook &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;9. CGHS/
+  ECHS/ ESIC/ Medi-Claim Card with Photo issued by State/ Central Govts./ PSUs &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;10. Disability ID Card/
+  handicapped medical certificate issued by the respective State/ UT
+  Governments/ Administrations/ Central Govt. &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;11. Photo ID Card/ Certificate
+  having address issued by Central/State Govt.&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+&lt;/table&gt;
+&lt;p class=MsoNormal&gt;&lt;span style='font-size:16.0pt;line-height:107%;font-family:
+"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;p class=MsoNormal&gt;&lt;span style='font-size:16.0pt;line-height:107%;font-family:
+"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;table class=MsoTableGrid border=1 cellspacing=0 cellpadding=0
+ style='border-collapse:collapse;border:none'&gt;
+ &lt;tr&gt;
+  &lt;td width=623 colspan=2 valign=top style='width:467.5pt;border:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:aqua'&gt;POR (Proof of Relationship)&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr&gt;
+  &lt;td width=274 valign=top style='width:205.3pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;The POR documents specification:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=350 valign=top style='width:262.2pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;1. It should contain the Introducer’s Full Name and a clear Photo&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;2. It should contain the applicant’s Full Name and a clear Photo&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;3. The relationship between the Introducer and resident should be clearly
+  mentioned&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;4. All the produced documents should be valid for at least the next 6
+  months&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr&gt;
+  &lt;td width=274 valign=top style='width:205.3pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;Acceptable document:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='font-size:16.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=350 valign=top style='width:262.2pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;1. Passport of Spouse/ Passport of Parents (in case of Minor) &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;2. Ration card/PDS Card&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;3. Medi-Claim Card with Photo issued by Centre/ State Govts./ PSUs &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;4. Pension Card&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;5. Birth Certificate issued by Registrar of Birth, Municipal Corporation,
+  and other notified local government bodies &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;6. Any other Central/ State government-issued family entitlement document
+  &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;7. Marriage Certificate issued by the government &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;8. Photo ID card issued by Central/ State Govt. like ARMY canteen card
+  etc. &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:
+  -.25in;line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;9. Discharge card/ slip issued by Government/ Private Hospitals for birth
+  of a child (only for child aged between 0-5 years) &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;
+  line-height:normal'&gt;&lt;span style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;
+  &lt;/span&gt;10. Self-declaration from the Head of Family (HoF) certifying the
+  relationship with the resident residing at the same address as HoF&lt;span
+  style='font-size:11.5pt;font-family:"Arial",sans-serif;color:#1D1C1D;
+  background:white'&gt; &lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+&lt;/table&gt;
+&lt;p class=MsoNormal&gt;&lt;span style='font-size:16.0pt;line-height:107%;font-family:
+"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;p class=MsoNormal&gt;&lt;span style='font-size:16.0pt;line-height:107%;font-family:
+"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;table class=MsoTableGrid border=1 cellspacing=0 cellpadding=0
+ style='border-collapse:collapse;border:none'&gt;
+ &lt;tr&gt;
+  &lt;td width=623 colspan=2 valign=top style='width:467.5pt;border:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:14.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:aqua'&gt;DOB (Date of Birth)&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr style='height:34.7pt'&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt;height:34.7pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;The DOB documents specification:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt;height:34.7pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;1. It
+  should contain Full Name, a clear Photo and DOB&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;2. It
+  should be valid for at least the next 6 months&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+ &lt;tr&gt;
+  &lt;td width=217 valign=top style='width:162.8pt;border:solid windowtext 1.0pt;
+  border-top:none;padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;b&gt;&lt;span style='font-size:11.5pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;Acceptable document:&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+  &lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center;
+  line-height:normal'&gt;&lt;span style='font-size:16.0pt;font-family:"Arial",sans-serif;
+  color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+  &lt;/td&gt;
+  &lt;td width=406 valign=top style='width:304.7pt;border-top:none;border-left:
+  none;border-bottom:solid windowtext 1.0pt;border-right:solid windowtext 1.0pt;
+  padding:0in 5.4pt 0in 5.4pt'&gt;
+  &lt;p class=MsoListParagraphCxSpFirst style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;1. Birth Certificate &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;2. Passport&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;3. PAN Card/e-PAN&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;4. Service photo
+  identity card issued by Central Govt./State Govt./UT Govt./PSU/Banks &lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;5. Photo ID card having
+  Date of Birth, issued by Recognized Educational Institution&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;6. Valid School
+  Identity card/Identity Card issued by recognized educational institutions&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;7. Gas Connection Bill&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;8. Marriage Certificate
+  issued by the Government containing Name and address&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpMiddle style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;9. Registered Sale/
+  Rent Agreement&lt;/p&gt;
+  &lt;p class=MsoListParagraphCxSpLast style='margin-bottom:0in;text-indent:-.25in;line-height:normal'&gt;&lt;span
+  style='font:7.0pt "Times New Roman"'&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp; &lt;/span&gt;10. Telephone Landline
+  Bill/ Phone (Postpaid Mobile) Bill/ Broadband Bill&lt;/p&gt;
+  &lt;/td&gt;
+ &lt;/tr&gt;
+&lt;/table&gt;
+&lt;p class=MsoNormal style='margin-bottom:0in'&gt;&lt;span style='font-size:11.5pt;
+line-height:107%;font-family:"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;p class=MsoNormal style='margin-bottom:0in'&gt;&lt;span style='font-size:11.5pt;
+line-height:107%;font-family:"Arial",sans-serif;color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/p&gt;
+&lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center'&gt;&lt;b&gt;&lt;span
+style='font-size:16.0pt;line-height:107%;font-family:"Arial",sans-serif;
+color:#1D1C1D;background:yellow'&gt;Sample acceptable identity card&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center'&gt;&lt;b&gt;&lt;span
+style='font-size:16.0pt;line-height:107%;font-family:"Arial",sans-serif;
+color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center'&gt;&lt;b&gt;&lt;span
+lang=EN-IN style='font-size:16.0pt;line-height:107%;font-family:"Arial",sans-serif;
+color:#1D1C1D;background:white'&gt;&amp;nbsp;&lt;/span&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class=MsoNormal align=center style='margin-bottom:0in;text-align:center'&gt;&lt;b&gt;&lt;span
+lang=EN-IN style='font-size:16.0pt;line-height:107%;font-family:"Arial",sans-serif;
+color:#1D1C1D;background:white'&gt;&lt;img width=450 height=299 id="Picture 1"
+src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAVIAAADhCAYAAACa/D2AAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAACxMAAAsTAQCanBgAAP+lSURBVHhe7P0HuBVVuq4N9/n+/+zzn7B3R7vtoN22Oeecs4KKomKOmHNEzBhBQRElKyAqRlAJKooREBElS845Z1h58f7P/VaNWjXnqjnXYmHv/X3X57h4qblqxKoa465nhKr6VUW52S/2i/1iv9gv1jArL9u8+ReQ/mK/2C/2i22F/QLSX+wX+8V+sa20X0D6i/1iv9gvtpX2C0h/sV/sF/vFttJ+Aekv9ov9Yr/YVtovIP3FfrFf7BfbSvsFpGmryNj3/xb7Vx/7/5vPbX3sl/Pz/2jbepBSAWSVWGVs4e+f1TY3zMrrsurIyqqsoqTMKksrov3k6ceSH/7ntDhvt7BP5aAMZZUqS3m0LRjn57GKsgqr2FTi5yA6bzrujHBbYxUcC8dGHn5M2eHqZZ6GjPPhZc06L5vrnZefb/8dznEDzMujNBpYX7zuefxQ50gvHGMRi48hihdbso8wqf21LM/f49UVJ8+y8i9m9c0jPi+ZfsE8TB15F/PPyyOTb/W0BoNUEaMKuHG9VWnH5s3V8ihViWS2WVbAEW6LrcqsWke6xaaCVpUVMflXbrLNlSVmZets87qFtnnTCh1HiW0uXWtWusb9PZ260uO4FW/LTHmXx1a23vPcXLLGqtcvVTlWqzyLbPPahTrZG2QqB3nINpdv3DIr2xCln1j8N/npGKs3LLPqlTOU56po/8aVkV9OnDrM0ypk6616zTyrXj0nPjblU56RRr1MZS9RmjpPm0t1zbzM2pccL+dSf8uvmnNYItP5yzkfObbJqjcut83rl6kO6DxnXqdCpuuhNEzH5/lsWKrro/1Z9aOgUQfLdJ11rUtWxXWMusQ1V9r416rXKVPYzapHVq02QlshvLdDpU27qdWWgqmNEo9wxK2WavC8tK2PIz7xiO95FWnzOPJU2ps9D8Ur5kK6VUXKovQ8LSyLN14+lFCBslEejx/lQRB2VVaKa4JvhQBbrqj53CtkWwxSAIpxN/NKS2NXBfeTtFGVWhXbT4QqGpU9ulAqLJXUD0qlTVxc+rAtaFzojEpUp6nAmZW3gHl4DlINLAdiaohqbA5WD6fjIf103C0GadQIE9jQEDcBMMEhbuAAoHrjCu1TvsCD34TBX2m4edg6DLAECLH1vLhWSivAk2NkqzyqV8/TfuUV9ge/YpYDzjwjD52/6pUzBdIlUb7A2suWkVZ9jDIp3erV86PzEs4H+QHZ5Lg4j3nnI8OqudYlK6M6ivk1KmRca0GIm6+ui1HPKQ91hhtxVV7dqNNoXCrnRsGcG7fDWPtq1ecM26y6qDQc4hwLZaN+ZrajlNHq4uNm62Wul4sB5cdI/hmQyncePm5bxRzlqpQoq8WJPAcPAleynOLWQDbDBVCTTr7Tvs06rqrKAFPAqstTh20RSMtKq62srNoziQ40nMQARG3YqqAOBCmd6CLp5ABZ7rj85oLTkIAPJ4OL73fP1EUJtwi3/ySQBqOxhAYl84ZJhVOZ8du8QQpGx+bKgTziypzb2LKMBijjnOj8mDd6VJPSB3JZjT6oVhQWylENBkBUS0FVr1ssP8VT2lG4vLjByjBBJQZoNefeQaNrFMCUWAxNDyuorgFUCu/li/2yjOudhifmoBbkUHwBbOSpY6heNTu6ScQ3jFrp1csUj3x1/vx8rNE14lyiEOsJ0MQ4h6hklckwrn3OtUtdQ+XrN1UAym/2UZfJU8fp4fjbG7PSKWj4x/WhAlN8nR8AXXedV53T1tUo5VdvCmWd226KmIBFGThfdSrE4MiT9kDZSaMuxzHQ3jmXdYWPYQvEFDjal+9IA3+Ov1B6AZKFjgk2cexZ/nF5Q9qbdS4rxLv6wLTeICUxQFpVzUHW42IljrBxHCoNF4FGEHeh/WLSoNRwOUneEKRavCKGeJhXnGChMtVlKrhX2C20WupSf3NxvHGpsnODAKTyc+CsWaCtGhDxPFxGfCq8jjtqfDQW/eY8eEOuZ6MnPwwY0UWmOyhgJWCsFSdOly5uCMP5DRDybREDhH4D0fVRGoA88suImwYp+Tg8ua76HfYHo/xSX65+1y2Juvv1KU+WkS/5qc5Ur5qjMipfv6nU85zmmcdfq+uptGtdRwE/ugHG1y/tFwxF5eWRQvT6VKgOKm3SowsPRFGh1FnOD6qdeEXq+maUq8cnrtJSWG5I3lYKwlT7STfU09Ct1XF7uoUccf044jLV6bYgfJK28ud3IUc6DsjC6W3meDzPLIiqBx3K5FzJdQ5wrkue32bxrry00tlXDKj1AikJlJZUWUVFONBCF6oexgVDwfkdV1tgF99V/SBpHA5VHZROnKs/VUz+9spNxUlVqFwjvfTfSi+puFtgtUCYZw5LGb9pyCqjbwEECk5dvChs3Fjo/qmBBHj6eKfDFRWU3aCLGufIfwdFJsgl3XH9HYepDuCUevJxReLVG1hKx49Jv+M8OC7vCtYKG8LEAA3QdnCSTgzQtJE+8ejyr54b3Zzy0yxqik8e5EW+7COv5Jj1u0EwVRzSCjc8rqP2+zXkb1egNdevtkXXPOqN6VpTD3PqF/GUHn4BoN7A8/wDNHLqs0zhPV3K4ACN94cuPteJ/fltVGG4CUegITz7CSPjmBEv+YAhTAjvcMrzr+XkT5n9eMijjvCEqQOO7mL1XFBlkk8oZ1YZ3Z/4WWWK45IHx5vvVMbqyp8JpFGXXpI4KYS24QJtkQFPLkqeOVjjShMgG1eM5K4bKomPyapCq0JVMzmEEnRgYvHJCumwZd+WWl0gTVu4u1PBaYBh3FFWvXKWd2EdojRGB2h+GlmNuQ5LYBIbDZdzA0DUIKqWTbMq4EQXF6A4POsL0GCKlw8/0o+PzyePgGaAORB3BapyePiM+FkWgEiawAf1y77MMsWma+7DAg5M0gh+KgvnB6W7YoZgpjA6x1sMVFe0Uqe6OaFyozFQXb+iAE2Z1x+FJU5cV71eJQAFgvG+LFO9DTelBBBx/coFaFzHU+bXh96SN1O1OeATykUYb4f57VdtG2WcdoR1yNUHoHKEI3xdyhLnXWiFQ0EWC4ufp0m4AmXwMJwPhcly8vehhUL+fn7xy0jfmRLFYwLKxaR2ZVm9QJqrRmPHATTEMi5+UQuQpYKFCuqVUL9pxFRMKpkaMY3bwUs8r9Chsiqsb3UwXlHjbSHzfOLKVx8LDdWVH1CIFRENHbDgR+NeM1eNknHWuJF5/FQDrq8l4IjNoaV8gAsKDfOyrImUqqu9GKacs/z4mVYAhL5fBkTXL47S5ncC0IZYnCYw1Q3Au/phX1Je/tYxAUfAi1+tMsfmaekcOGjjcFnnsZBxnkoUj2Ojiw4MHaBbUi8UVg14s+rk5o1MBMWCgLqVVedyjPpZGg2rUJ+oL7GYiNpFoTbEfsUNYAEgnh9+iJNiAkj+3OiT7rG2heCVdtWKS3jWD/G7mCM9lcUVM3kWdApH/n68gDzL0VVXnoQplBbH5OciIw3KUhCwStv9lH7sqquqrWRTZUFVWidIUaMlAmk0NppyORdhC8wvNid9Cy1AMNlyoKnfnLAATlU6VxPMgiq8Q8ZnZOMwVGqvYHEa+WDFL7NxYLGfGlyiOByYcaOl4bupQaoBJGrIG6egQTgaNg1U8AGqEeC09fCpBp1phI9hEcDt6kxbYOPQiMvAb8Y2UfEhHIAhXDpMppF+BvD8WHU+UZ8xQL1rzrgiYUL8WnHraZ6+tox5Mkzi+5Wvq1ZuEPo7p5yFjOOL6wHp8HfR8xtfB79G1Bdtw37lbag8/V27PmSZ6oji+TBOfK6SG3y6nmWa6iJ1VOlwfX1SizS9HdSj7RCfcq9dpLjKHyhltcPEYn/Gdhlz101YO7yJF3XEIb8Klbkg7FJOYXySyhVekfSVbjQZpLQLhSNv50ChMAGyCpN1MyAPyu3x85zCO+jz/OiNl8VjpVmcrBOkJSVI2gKzaRyQ75OFC1KXcdLTF76+5icuVLZClhGGOwsNcc0C72J7Q1yvSkbj0Anjb4chYR2q5MfB5zUMtjQkNTZvIMRTo/ffcbgEmgUt9qdBK37oGrN12AEA0nHLT4u/1dAdZmqcrjwBaAzmOm1dBJVVgl6Iz5a0C4SPIIbFeQIyJolQavyd+OtY2AfstPUlTkCeeKkw9Tflr/jVq2ZZNYB2ha20AF1mWYubl8fPk9Lw65R9Xqs5Jg+nv3PCCMiMe+tmFN1k4/pQy9gPQEkvuiEEPz9nOrZa9TMx6m6Iz7EyJBDNC3CTcrgWBKn2E98BTA9N9RpVr5uou6x2GIx27cpVRjm5ARR1aufk54qtDijivBtP2RSe/Aq6KN1ICRYJBz88jMqd5fyYOJfyLwBRHw/NVKlAXOcuC7AqW3lpuVRpdve+TpBuUsTS9aoY3FUpPHeUuIL6iQyVKP+k+knjbxm/g/1LQZphXvFVvrClslDRASmwosJx91Zj8aECQc3hSHjie8XW31RsGoKbfpfHx52yukGab3EjFqB8ORCz60rfocpv0sS8YQowNPItVmZYABoNVH+rgTNpRJ6eVlIe5ZMTR+YAXRGPX9YGaI1FYR3WK2f5efR9Af6ZcQoYx8jNhYlG0tS22hesA7lQvi2xqAyk4cMGybnXlvxI1xW9wibnIt8UnnOi8kTKtKY+Jb8V3+uG0rOy3DDk4TD2epxRl0mT+A5QxUn5+RpR6qHltx21OW76hGcWnzDE2czCd235m/aWbn9uEbQoB/Urgo72xzCL2nKG8zi0RfIgfBFHHrAC6GWBKe0oI2XxcDAjw3l6DAvoeAvlrf0oTZ+9z3LxMWfG9/Qpa0Zcz7dMsKywTRsrMrv3RUGKjN20sdJKN1EZdKHjE+MVnbszB16mikgXmorAycCP7giFJg4Xk4Indwdtk0rAtp6WVfnqYymA1pj2JYDlro/KVGOhUXn3RjAFGHQJUQOlajxUco+nNHMaUY1tOUixuKHzm+1GxgkZlhDg6JZLSUeKSuUJDT2sC6235YNMf2tf9frFgpTAQiP3he0Cl5cF8ABthgKwCGh1AhEg+VYWDylUr5yj3zqWWmXItwhSnh/A9psFcaL9nBP383Om8mUeZx2mc+pAdiiqJ+DHRJmVR53XLvL3Y1K9qIGpFIzSdoBi1KUC9SOCK8DT1oeTaGj6W8fj9Ys0s+qw1/9InUbtJmo7DsE0QPPbFPt0jBHI1O68HQpaoQ57nBRoCcNxqqeTAz/8HHQqb5aSy3ObVY4orNJI2n22A54OfcpeyJE/ACXNAo483b9QOp6P/Dn+fOfHxzmr7bfZz7POlcJUVFTZxg1lmd37OkG6cUO5d+2VUpRh+sSEC8eFBExYXDkjyFJ51Qi54DqIaCE7M5GEZV/q4odJJX4XMsJvqWWCNM8oCw0gNITQeIOCURhXiFJx0bgmcWqn3TCQ5kEBqLhCUn503Wn4G+gqC3zcpBx0ipeOU6cBpHxwyYI/6bIWdiNQRQHGICvBYtBkxc83L3ds/M045yqB1NWp/i5UjnCsDu0ieVI2QMYkV0NgShyZr11lEog0/ZrV87qpnvuwA+fHgSij+650IoDW1IVM46bNsTG0BEwBKOYihfqqdpZff8N+hfHJVFef1DXiAVDVwdCGMoy64/UUR5sM7RRRRFv2Np0y7fdzn45TDFA5Tun5MdQd3h/cIVwxhYmjm+9d8fjvLBfyJP9aLi4TN65MqMflyCiDK9sYojhAun5d6VaAdJMuZgLSlIULlgYgxMfC3+Fiq0KEBuEzkigBlIcalz/vTneWLgwVpxBQ0xUr+V2H5cEuMTUeVwGq2FF3Xb9pDHEFdXiiNtjS0GgAqTFJB4QapB9fnOZWgTSBiaDmXfwoH0/TASRj/FEK2bu8+NXbCgAsMfnTs4jVYPWyKf44Z+JXK3wB49ykzfdH8X02nqEE388+Gb9Ru35eASjHXUd+KOi183VTUfhw7upjpOvnVobaR/U7ELf0ulE3SqO43FhVpuj6F6hnOaYwqmM+7qv4VqV9Xk/rUZ8dwiq3rlH0GKn2ZbWRHFM7ov7z22/8cZz8dpxjtHMma6I2GwFX++tynhfpa5sJtBrnXXjC0s6LuM0oRNLz5CRgNi+yD2d/awPnjzRbsdQqJo7Q+dD5L+Q4jnDMGS5RsVnH58eT8lNaFaWltn59WeYyqC1QpOFEp4zMkotWwLIg6xVDlSjcVXWxHagsZZKfN2bWiKJsuftSeUJ3iIpB3FDBQhcp/J1vDlJgJyM/Kr4acKQi6E4BT6UdKnpS6fMbFw2IRqffNIa46+2/aVR0PWms7q+Gm46X/E6bIOCNW+k4SJRWgIw3/gxIBBjovNDdr/K1kkCVOFghsMgvgCjHlA75o7qTMshQkPzN2KS/yIU8SaNQOrFR/kJGmiznCaqTmwLnLVGgGellGcdCeMVzZUo5fXikkKHkdUycJwe10vBzr20om+/Lukb5pngK7z0DxWHYhXPj9S+pN0WMm7XiJzdwV6JF6m4w6jBtI9RfHVOOWClotBfaDzcP5jhofxmCKMdon1Ky1AnyqcuRnh+D8iN+MSf/mqeL6ghbVW1Vqz62ysXP6DC+scr1x1vlusNs+PzWNmr9Givt0caWNtvDysd8o8CbrXLuXCsZ0F/nSOcLly5XhnO16TeZjHIErpEGjrIqrYqyctsgkG6xIpWnRywtoXAZF6A+IM2yUEHSEOS3/63fDj5VMgemIOtLd3QHB25cYMaopKCiChbDOJ0OW/w8LaVD5aPiCgQROIEqeVDB0/BMWyEAxub+cRgaLI1UlZ2F4q6+aLjBL4kH6GiMOh4qtzdi+ReDZ76RBuBw4AE/YLAqAh5/J2Hy0kpDkDgOywAyABMDBQNWMbB8jJbJIy+vLITJMi9LIZM/QFO+LJZH9XreXr5U2eplcfnUbfWeAWUL5zrneJUv54R8iJf251wrDpNuVUF967rXXKu0cS6Vnr8vQsfgcXXt/Xqpfim97Doko54pXPRkFDDkpk29pas+389NTptIWxAbQBQVqjrux4QSxj+/XQXz7jh5EI9ybIqGBYqBFD/iUWa16+icFQGp0nFlSbsDvkVVqPxIkzbpYYs4laN6/jAr//phK//sCquc8qxVbXrGylf/Tytb8SsB9XqF2WCbPuppqx65wkoGPWKlX99lG16929Y89ICtXbzc1pfqRuBqskBenCNXxDrufAfTOKZwPIThXEtI0rVvEEiJQMSSQl37et0VMyxAr6DJPwAxGBfBwQkE4wouCPnz1VJn+HklRyFQ2fTbF79TmbxSx/HTlbyo1QHSHAtQjeGF0kOxAg9eJgH8gYmDLzREjLhxnC2yGDxpACntqlUALzoHEVTlH/KIz4k3EABK+dgX4mdZgGAM/Sq65nRLied5p/JPh08s3kd81C2TZgDcFSJl4LfKEUDXECN9bf3Gxd+cH8rnPQbSVRlrnb+Uyd+Vsd8kFDa57vGWG50fS7hu+AVTGIWv8lUKdLlD/WJLPQWgAiUQ5e90/aK+rouWZXmvLa+uk76vIWWbdLNj4zip1zntLwYAYREPoQcXix3qgIfPAimQo8zEddgGvwIgkp+DKg2cQs7DUm6FDQqviKue85GVvrKflbzwJyvp8Ff9PtgqZ7SVGj3Fyub/u1VN28Wqp55q1QsftIopL9uGHgfbuud+Y5WvHWHzfxpuF7w6zs7sMtJmr9CxZDngz/nKKrefq/QxaUtYzoVcRXnl1o2R/uwgzYdkvUxxuCChslIxuNNj3DlpBFRMGrsaKHd/BvWjYQGF9wYtuAJi0kinlWmhQdXX4vDeOOMGTuNDgQEfZuMBKt1R/AhLHli6YdfL8gCWmPYrbX/v50rGI8kfRQYIBRUAWpeqTJsfQzD9rXSi2XOlFbrK6bKkw7KNwzlAHVYKn/hHcZLlUp6Wjo1jCOnV2wRD1sf60IGOz5Wj8ql13goZNxqlsXp+dAPkWmq/z+pzDITJudZ5Rtx1i6N6Q71S+KhOCqDyr123co1jiOo49VLhgSSWD9BgtB/vsck/tEGvy4Be7cGFSEab8zT129sukB</t>
   </si>
 </sst>
 </file>
@@ -17768,10 +18136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1689"/>
+  <dimension ref="A1:M1690"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1251" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1257" sqref="F1257"/>
+    <sheetView tabSelected="1" topLeftCell="A1690" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1693" sqref="F1693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -87026,6 +87394,47 @@
         <v>23</v>
       </c>
     </row>
+    <row r="1690" spans="1:13" ht="409.5">
+      <c r="A1690">
+        <v>1500</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>2380</v>
+      </c>
+      <c r="C1690" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1690" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1690" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1690" s="16" t="s">
+        <v>2382</v>
+      </c>
+      <c r="G1690" s="26">
+        <v>10006</v>
+      </c>
+      <c r="H1690" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1690" t="s">
+        <v>2381</v>
+      </c>
+      <c r="J1690" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1690" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1690" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1690" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated template.xlsx file for reject mail/sms
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF95B5C-677F-480A-9B28-16C4BD007B83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91333B55-4AC8-4F33-9FB9-D7615DD6493B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$K$1807</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$K$1809</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16307" uniqueCount="2444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16305" uniqueCount="2442">
   <si>
     <t>id</t>
   </si>
@@ -9068,37 +9068,10 @@
     <t>vid-card-download-failure_SMS</t>
   </si>
   <si>
-    <t>Dear $!name_eng, 
-Your request for UIN for Registration ID: $!RID has been rejected by the Supervisor. Please visit your nearest Registration office for further details.
-Thank You,
-MOSIP</t>
-  </si>
-  <si>
-    <t>Dear $!name_eng, 
-Your request for UIN for Registration ID: $!RID has been rejected by the Supervisor. Please visit your nearest Registration office for further details.</t>
-  </si>
-  <si>
     <t>Address line2</t>
   </si>
   <si>
     <t>mosip.address.line2.template.property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">عزيزي $! name_ara ،
-طلبك للحصول على UIN لمعرف التسجيل: $! تم رفض RID من قبل المشرف. يرجى زيارة أقرب مكتب تسجيل لمزيد من التفاصيل.
-شكرا لك،
-MOSIP
-</t>
-  </si>
-  <si>
-    <t>عزيزي $! name_ara ،
-طلبك للحصول على UIN لمعرف التسجيل: $! تم رفض RID من قبل المشرف. يرجى زيارة أقرب مكتب تسجيل ل</t>
-  </si>
-  <si>
-    <t>प्रिय $!name_hin,
-पंजीकरण आईडी के लिए यूआईएन के लिए आपका अनुरोध: $!आरआईडी पर्यवेक्षक द्वारा अस्वीकार कर दिया गया है। अधिक जानकारी के लिए कृपया अपने निकटतम पंजीकरण कार्यालय में जाएँ।
-धन्यवाद,
-मोसिप</t>
   </si>
   <si>
     <t>प्रिय $!name_hin,
@@ -9126,9 +9099,6 @@
   </si>
   <si>
     <t>Template for Supervisor Reject Email Subject</t>
-  </si>
-  <si>
-    <t>UIN Request Rejected</t>
   </si>
   <si>
     <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
@@ -10192,6 +10162,20 @@
 We are pleased to inform you that] National Identification Number (NIN) $!MASKEDNIN has been renewd for your application with Registration ID $!RID.
 Please pick up your ID card to access the full details.
 Thank you.</t>
+  </si>
+  <si>
+    <t>Your request for NIN for Registration ID: $!RID has been rejected by the Supervisor. Please visit your nearest Registration office for further details.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dear $!surname_eng $!givenName_eng,
+Your request for NIN for Registration ID: $!RID has been rejected by the Supervisor. Please visit your nearest Registration office for further details.
+Thank you </t>
+  </si>
+  <si>
+    <t>NIN Request Rejected</t>
   </si>
 </sst>
 </file>
@@ -10538,7 +10522,7 @@
   <dimension ref="A1:K1809"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1809" sqref="M1809"/>
+      <selection activeCell="F1740" sqref="F1740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11054,7 +11038,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2431</v>
+        <v>2425</v>
       </c>
       <c r="G15">
         <v>10003</v>
@@ -11089,7 +11073,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>2432</v>
+        <v>2426</v>
       </c>
       <c r="G16">
         <v>10003</v>
@@ -11124,7 +11108,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>2434</v>
+        <v>2428</v>
       </c>
       <c r="G17">
         <v>10003</v>
@@ -11159,7 +11143,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>2433</v>
+        <v>2427</v>
       </c>
       <c r="G18">
         <v>10003</v>
@@ -13364,7 +13348,7 @@
         <v>13</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>2435</v>
+        <v>2429</v>
       </c>
       <c r="G81">
         <v>10003</v>
@@ -13469,7 +13453,7 @@
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>2435</v>
+        <v>2429</v>
       </c>
       <c r="G84">
         <v>10003</v>
@@ -13574,7 +13558,7 @@
         <v>13</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>2436</v>
+        <v>2430</v>
       </c>
       <c r="G87">
         <v>10003</v>
@@ -13662,7 +13646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1135</v>
       </c>
@@ -13679,7 +13663,7 @@
         <v>13</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>2436</v>
+        <v>2430</v>
       </c>
       <c r="G90">
         <v>10003</v>
@@ -13802,7 +13786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1137</v>
       </c>
@@ -15167,7 +15151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1154</v>
       </c>
@@ -15412,7 +15396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1156</v>
       </c>
@@ -71027,7 +71011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1729" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1729">
         <v>1554</v>
       </c>
@@ -71043,8 +71027,8 @@
       <c r="E1729" t="s">
         <v>13</v>
       </c>
-      <c r="F1729" t="s">
-        <v>2285</v>
+      <c r="F1729" s="1" t="s">
+        <v>2440</v>
       </c>
       <c r="G1729">
         <v>10003</v>
@@ -71062,7 +71046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1730" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1730">
         <v>1555</v>
       </c>
@@ -71078,8 +71062,8 @@
       <c r="E1730" t="s">
         <v>13</v>
       </c>
-      <c r="F1730" t="s">
-        <v>2286</v>
+      <c r="F1730" s="1" t="s">
+        <v>2440</v>
       </c>
       <c r="G1730">
         <v>10003</v>
@@ -71102,10 +71086,10 @@
         <v>1580</v>
       </c>
       <c r="B1731" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="C1731" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="D1731" t="s">
         <v>12</v>
@@ -71113,9 +71097,6 @@
       <c r="E1731" t="s">
         <v>13</v>
       </c>
-      <c r="F1731" t="s">
-        <v>2287</v>
-      </c>
       <c r="G1731">
         <v>10006</v>
       </c>
@@ -71123,7 +71104,7 @@
         <v>288</v>
       </c>
       <c r="I1731" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
       <c r="J1731" t="s">
         <v>17</v>
@@ -71132,7 +71113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1732" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:11" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1732">
         <v>1558</v>
       </c>
@@ -71149,7 +71130,7 @@
         <v>13</v>
       </c>
       <c r="F1732" t="s">
-        <v>2289</v>
+        <v>2438</v>
       </c>
       <c r="G1732">
         <v>10003</v>
@@ -71183,9 +71164,6 @@
       <c r="E1733" t="s">
         <v>13</v>
       </c>
-      <c r="F1733" t="s">
-        <v>2290</v>
-      </c>
       <c r="G1733">
         <v>10003</v>
       </c>
@@ -71219,7 +71197,7 @@
         <v>13</v>
       </c>
       <c r="F1734" t="s">
-        <v>2291</v>
+        <v>2439</v>
       </c>
       <c r="G1734">
         <v>10003</v>
@@ -71254,7 +71232,7 @@
         <v>13</v>
       </c>
       <c r="F1735" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
       <c r="G1735">
         <v>10003</v>
@@ -71289,7 +71267,7 @@
         <v>13</v>
       </c>
       <c r="F1736" t="s">
-        <v>2293</v>
+        <v>2288</v>
       </c>
       <c r="G1736">
         <v>10003</v>
@@ -71324,7 +71302,7 @@
         <v>13</v>
       </c>
       <c r="F1737" t="s">
-        <v>2294</v>
+        <v>2289</v>
       </c>
       <c r="G1737">
         <v>10003</v>
@@ -71359,7 +71337,7 @@
         <v>13</v>
       </c>
       <c r="F1738" t="s">
-        <v>2295</v>
+        <v>2290</v>
       </c>
       <c r="G1738">
         <v>10003</v>
@@ -71377,7 +71355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1739" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1739" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1739">
         <v>1565</v>
       </c>
@@ -71394,7 +71372,7 @@
         <v>13</v>
       </c>
       <c r="F1739" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
       <c r="G1739">
         <v>10003</v>
@@ -71412,15 +71390,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1740" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1740" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1740">
         <v>1566</v>
       </c>
       <c r="B1740" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C1740" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="D1740" t="s">
         <v>12</v>
@@ -71429,7 +71407,7 @@
         <v>13</v>
       </c>
       <c r="F1740" t="s">
-        <v>2298</v>
+        <v>2441</v>
       </c>
       <c r="G1740">
         <v>10003</v>
@@ -71438,7 +71416,7 @@
         <v>58</v>
       </c>
       <c r="I1740" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1740" t="s">
         <v>17</v>
@@ -71452,10 +71430,10 @@
         <v>1567</v>
       </c>
       <c r="B1741" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C1741" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="D1741" t="s">
         <v>12</v>
@@ -71464,7 +71442,7 @@
         <v>13</v>
       </c>
       <c r="F1741" t="s">
-        <v>2300</v>
+        <v>2294</v>
       </c>
       <c r="G1741">
         <v>10003</v>
@@ -71473,7 +71451,7 @@
         <v>2253</v>
       </c>
       <c r="I1741" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1741" t="s">
         <v>26</v>
@@ -71487,10 +71465,10 @@
         <v>1568</v>
       </c>
       <c r="B1742" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C1742" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="D1742" t="s">
         <v>12</v>
@@ -71499,7 +71477,7 @@
         <v>13</v>
       </c>
       <c r="F1742" t="s">
-        <v>2301</v>
+        <v>2295</v>
       </c>
       <c r="G1742">
         <v>10003</v>
@@ -71508,7 +71486,7 @@
         <v>81</v>
       </c>
       <c r="I1742" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1742" t="s">
         <v>32</v>
@@ -71522,10 +71500,10 @@
         <v>1569</v>
       </c>
       <c r="B1743" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C1743" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="D1743" t="s">
         <v>12</v>
@@ -71534,7 +71512,7 @@
         <v>13</v>
       </c>
       <c r="F1743" t="s">
-        <v>2302</v>
+        <v>2296</v>
       </c>
       <c r="G1743">
         <v>10003</v>
@@ -71543,7 +71521,7 @@
         <v>1171</v>
       </c>
       <c r="I1743" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1743" t="s">
         <v>939</v>
@@ -71557,19 +71535,19 @@
         <v>1570</v>
       </c>
       <c r="B1744" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1744" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1744" t="s">
         <v>2297</v>
-      </c>
-      <c r="C1744" t="s">
-        <v>2297</v>
-      </c>
-      <c r="D1744" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1744" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1744" t="s">
-        <v>2303</v>
       </c>
       <c r="G1744">
         <v>10003</v>
@@ -71578,7 +71556,7 @@
         <v>880</v>
       </c>
       <c r="I1744" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1744" t="s">
         <v>549</v>
@@ -71592,10 +71570,10 @@
         <v>1571</v>
       </c>
       <c r="B1745" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C1745" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="D1745" t="s">
         <v>12</v>
@@ -71604,7 +71582,7 @@
         <v>13</v>
       </c>
       <c r="F1745" t="s">
-        <v>2304</v>
+        <v>2298</v>
       </c>
       <c r="G1745">
         <v>10003</v>
@@ -71613,7 +71591,7 @@
         <v>1372</v>
       </c>
       <c r="I1745" t="s">
-        <v>2299</v>
+        <v>2293</v>
       </c>
       <c r="J1745" t="s">
         <v>990</v>
@@ -71627,10 +71605,10 @@
         <v>1572</v>
       </c>
       <c r="B1746" t="s">
-        <v>2305</v>
+        <v>2299</v>
       </c>
       <c r="C1746" t="s">
-        <v>2305</v>
+        <v>2299</v>
       </c>
       <c r="D1746" t="s">
         <v>12</v>
@@ -71639,7 +71617,7 @@
         <v>13</v>
       </c>
       <c r="F1746" t="s">
-        <v>2305</v>
+        <v>2299</v>
       </c>
       <c r="G1746">
         <v>10006</v>
@@ -71648,7 +71626,7 @@
         <v>288</v>
       </c>
       <c r="I1746" t="s">
-        <v>2306</v>
+        <v>2300</v>
       </c>
       <c r="J1746" t="s">
         <v>17</v>
@@ -71662,10 +71640,10 @@
         <v>1573</v>
       </c>
       <c r="B1747" t="s">
-        <v>2307</v>
+        <v>2301</v>
       </c>
       <c r="C1747" t="s">
-        <v>2307</v>
+        <v>2301</v>
       </c>
       <c r="D1747" t="s">
         <v>12</v>
@@ -71674,7 +71652,7 @@
         <v>13</v>
       </c>
       <c r="F1747" t="s">
-        <v>2307</v>
+        <v>2301</v>
       </c>
       <c r="G1747">
         <v>10006</v>
@@ -71683,7 +71661,7 @@
         <v>288</v>
       </c>
       <c r="I1747" t="s">
-        <v>2308</v>
+        <v>2302</v>
       </c>
       <c r="J1747" t="s">
         <v>17</v>
@@ -71697,10 +71675,10 @@
         <v>1574</v>
       </c>
       <c r="B1748" t="s">
-        <v>2309</v>
+        <v>2303</v>
       </c>
       <c r="C1748" t="s">
-        <v>2309</v>
+        <v>2303</v>
       </c>
       <c r="D1748" t="s">
         <v>12</v>
@@ -71709,7 +71687,7 @@
         <v>13</v>
       </c>
       <c r="F1748" t="s">
-        <v>2309</v>
+        <v>2303</v>
       </c>
       <c r="G1748">
         <v>10006</v>
@@ -71718,7 +71696,7 @@
         <v>288</v>
       </c>
       <c r="I1748" t="s">
-        <v>2310</v>
+        <v>2304</v>
       </c>
       <c r="J1748" t="s">
         <v>17</v>
@@ -71732,10 +71710,10 @@
         <v>1575</v>
       </c>
       <c r="B1749" t="s">
-        <v>2311</v>
+        <v>2305</v>
       </c>
       <c r="C1749" t="s">
-        <v>2311</v>
+        <v>2305</v>
       </c>
       <c r="D1749" t="s">
         <v>12</v>
@@ -71744,7 +71722,7 @@
         <v>13</v>
       </c>
       <c r="F1749" t="s">
-        <v>2311</v>
+        <v>2305</v>
       </c>
       <c r="G1749">
         <v>10006</v>
@@ -71753,7 +71731,7 @@
         <v>288</v>
       </c>
       <c r="I1749" t="s">
-        <v>2312</v>
+        <v>2306</v>
       </c>
       <c r="J1749" t="s">
         <v>17</v>
@@ -71767,10 +71745,10 @@
         <v>1576</v>
       </c>
       <c r="B1750" t="s">
-        <v>2313</v>
+        <v>2307</v>
       </c>
       <c r="C1750" t="s">
-        <v>2313</v>
+        <v>2307</v>
       </c>
       <c r="D1750" t="s">
         <v>12</v>
@@ -71779,7 +71757,7 @@
         <v>13</v>
       </c>
       <c r="F1750" t="s">
-        <v>2313</v>
+        <v>2307</v>
       </c>
       <c r="G1750">
         <v>10006</v>
@@ -71788,7 +71766,7 @@
         <v>288</v>
       </c>
       <c r="I1750" t="s">
-        <v>2314</v>
+        <v>2308</v>
       </c>
       <c r="J1750" t="s">
         <v>17</v>
@@ -71802,10 +71780,10 @@
         <v>1577</v>
       </c>
       <c r="B1751" t="s">
-        <v>2315</v>
+        <v>2309</v>
       </c>
       <c r="C1751" t="s">
-        <v>2315</v>
+        <v>2309</v>
       </c>
       <c r="D1751" t="s">
         <v>12</v>
@@ -71814,7 +71792,7 @@
         <v>13</v>
       </c>
       <c r="F1751" t="s">
-        <v>2315</v>
+        <v>2309</v>
       </c>
       <c r="G1751">
         <v>10006</v>
@@ -71823,7 +71801,7 @@
         <v>288</v>
       </c>
       <c r="I1751" t="s">
-        <v>2316</v>
+        <v>2310</v>
       </c>
       <c r="J1751" t="s">
         <v>17</v>
@@ -71837,10 +71815,10 @@
         <v>1578</v>
       </c>
       <c r="B1752" t="s">
-        <v>2317</v>
+        <v>2311</v>
       </c>
       <c r="C1752" t="s">
-        <v>2317</v>
+        <v>2311</v>
       </c>
       <c r="D1752" t="s">
         <v>12</v>
@@ -71849,7 +71827,7 @@
         <v>13</v>
       </c>
       <c r="F1752" t="s">
-        <v>2317</v>
+        <v>2311</v>
       </c>
       <c r="G1752">
         <v>10006</v>
@@ -71858,7 +71836,7 @@
         <v>288</v>
       </c>
       <c r="I1752" t="s">
-        <v>2318</v>
+        <v>2312</v>
       </c>
       <c r="J1752" t="s">
         <v>17</v>
@@ -71872,10 +71850,10 @@
         <v>1579</v>
       </c>
       <c r="B1753" t="s">
-        <v>2319</v>
+        <v>2313</v>
       </c>
       <c r="C1753" t="s">
-        <v>2319</v>
+        <v>2313</v>
       </c>
       <c r="D1753" t="s">
         <v>12</v>
@@ -71884,7 +71862,7 @@
         <v>13</v>
       </c>
       <c r="F1753" t="s">
-        <v>2319</v>
+        <v>2313</v>
       </c>
       <c r="G1753">
         <v>10006</v>
@@ -71893,7 +71871,7 @@
         <v>288</v>
       </c>
       <c r="I1753" t="s">
-        <v>2320</v>
+        <v>2314</v>
       </c>
       <c r="J1753" t="s">
         <v>17</v>
@@ -71907,10 +71885,10 @@
         <v>1121</v>
       </c>
       <c r="B1754" t="s">
-        <v>2321</v>
+        <v>2315</v>
       </c>
       <c r="C1754" t="s">
-        <v>2321</v>
+        <v>2315</v>
       </c>
       <c r="D1754" t="s">
         <v>12</v>
@@ -71919,7 +71897,7 @@
         <v>13</v>
       </c>
       <c r="F1754" t="s">
-        <v>2322</v>
+        <v>2316</v>
       </c>
       <c r="G1754">
         <v>10008</v>
@@ -71942,10 +71920,10 @@
         <v>1253</v>
       </c>
       <c r="B1755" t="s">
-        <v>2323</v>
+        <v>2317</v>
       </c>
       <c r="C1755" t="s">
-        <v>2324</v>
+        <v>2318</v>
       </c>
       <c r="D1755" t="s">
         <v>12</v>
@@ -71954,7 +71932,7 @@
         <v>13</v>
       </c>
       <c r="F1755" t="s">
-        <v>2325</v>
+        <v>2319</v>
       </c>
       <c r="G1755">
         <v>10002</v>
@@ -71963,7 +71941,7 @@
         <v>50</v>
       </c>
       <c r="I1755" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1755" t="s">
         <v>17</v>
@@ -71977,10 +71955,10 @@
         <v>1109</v>
       </c>
       <c r="B1756" t="s">
-        <v>2327</v>
+        <v>2321</v>
       </c>
       <c r="C1756" t="s">
-        <v>2327</v>
+        <v>2321</v>
       </c>
       <c r="D1756" t="s">
         <v>12</v>
@@ -71989,7 +71967,7 @@
         <v>13</v>
       </c>
       <c r="F1756" s="1" t="s">
-        <v>2432</v>
+        <v>2426</v>
       </c>
       <c r="G1756">
         <v>10003</v>
@@ -72012,10 +71990,10 @@
         <v>1161</v>
       </c>
       <c r="B1757" t="s">
-        <v>2328</v>
+        <v>2322</v>
       </c>
       <c r="C1757" t="s">
-        <v>2328</v>
+        <v>2322</v>
       </c>
       <c r="D1757" t="s">
         <v>12</v>
@@ -72024,7 +72002,7 @@
         <v>13</v>
       </c>
       <c r="F1757" t="s">
-        <v>2329</v>
+        <v>2323</v>
       </c>
       <c r="G1757">
         <v>10003</v>
@@ -72047,10 +72025,10 @@
         <v>1113</v>
       </c>
       <c r="B1758" t="s">
-        <v>2330</v>
+        <v>2324</v>
       </c>
       <c r="C1758" t="s">
-        <v>2330</v>
+        <v>2324</v>
       </c>
       <c r="D1758" t="s">
         <v>12</v>
@@ -72059,7 +72037,7 @@
         <v>13</v>
       </c>
       <c r="F1758" s="1" t="s">
-        <v>2434</v>
+        <v>2428</v>
       </c>
       <c r="G1758">
         <v>10003</v>
@@ -72082,10 +72060,10 @@
         <v>1117</v>
       </c>
       <c r="B1759" t="s">
-        <v>2331</v>
+        <v>2325</v>
       </c>
       <c r="C1759" t="s">
-        <v>2331</v>
+        <v>2325</v>
       </c>
       <c r="D1759" t="s">
         <v>12</v>
@@ -72117,10 +72095,10 @@
         <v>1123</v>
       </c>
       <c r="B1760" t="s">
-        <v>2332</v>
+        <v>2326</v>
       </c>
       <c r="C1760" t="s">
-        <v>2332</v>
+        <v>2326</v>
       </c>
       <c r="D1760" t="s">
         <v>12</v>
@@ -72129,7 +72107,7 @@
         <v>13</v>
       </c>
       <c r="F1760" t="s">
-        <v>2322</v>
+        <v>2316</v>
       </c>
       <c r="G1760">
         <v>10008</v>
@@ -72149,13 +72127,13 @@
     </row>
     <row r="1761" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1761" t="s">
-        <v>2333</v>
+        <v>2327</v>
       </c>
       <c r="B1761" t="s">
-        <v>2334</v>
+        <v>2328</v>
       </c>
       <c r="C1761" t="s">
-        <v>2335</v>
+        <v>2329</v>
       </c>
       <c r="D1761" t="s">
         <v>12</v>
@@ -72164,7 +72142,7 @@
         <v>13</v>
       </c>
       <c r="F1761" t="s">
-        <v>2336</v>
+        <v>2330</v>
       </c>
       <c r="G1761">
         <v>10001</v>
@@ -72173,7 +72151,7 @@
         <v>153</v>
       </c>
       <c r="I1761" t="s">
-        <v>2337</v>
+        <v>2331</v>
       </c>
       <c r="J1761" t="s">
         <v>17</v>
@@ -72190,7 +72168,7 @@
         <v>190</v>
       </c>
       <c r="C1762" t="s">
-        <v>2338</v>
+        <v>2332</v>
       </c>
       <c r="D1762" t="s">
         <v>12</v>
@@ -72199,7 +72177,7 @@
         <v>13</v>
       </c>
       <c r="F1762" t="s">
-        <v>2339</v>
+        <v>2333</v>
       </c>
       <c r="G1762">
         <v>10002</v>
@@ -72208,7 +72186,7 @@
         <v>50</v>
       </c>
       <c r="I1762" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1762" t="s">
         <v>17</v>
@@ -72222,10 +72200,10 @@
         <v>1111</v>
       </c>
       <c r="B1763" t="s">
-        <v>2341</v>
+        <v>2335</v>
       </c>
       <c r="C1763" t="s">
-        <v>2341</v>
+        <v>2335</v>
       </c>
       <c r="D1763" t="s">
         <v>12</v>
@@ -72234,7 +72212,7 @@
         <v>13</v>
       </c>
       <c r="F1763" s="1" t="s">
-        <v>2433</v>
+        <v>2427</v>
       </c>
       <c r="G1763">
         <v>10003</v>
@@ -72257,10 +72235,10 @@
         <v>1682</v>
       </c>
       <c r="B1764" t="s">
-        <v>2342</v>
+        <v>2336</v>
       </c>
       <c r="C1764" t="s">
-        <v>2342</v>
+        <v>2336</v>
       </c>
       <c r="D1764" t="s">
         <v>12</v>
@@ -72278,7 +72256,7 @@
         <v>153</v>
       </c>
       <c r="I1764" t="s">
-        <v>2343</v>
+        <v>2337</v>
       </c>
       <c r="J1764" t="s">
         <v>17</v>
@@ -72292,10 +72270,10 @@
         <v>1253</v>
       </c>
       <c r="B1765" t="s">
-        <v>2344</v>
+        <v>2338</v>
       </c>
       <c r="C1765" t="s">
-        <v>2324</v>
+        <v>2318</v>
       </c>
       <c r="D1765" t="s">
         <v>12</v>
@@ -72304,7 +72282,7 @@
         <v>13</v>
       </c>
       <c r="F1765" t="s">
-        <v>2345</v>
+        <v>2339</v>
       </c>
       <c r="G1765">
         <v>10002</v>
@@ -72313,7 +72291,7 @@
         <v>50</v>
       </c>
       <c r="I1765" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1765" t="s">
         <v>26</v>
@@ -72327,10 +72305,10 @@
         <v>1253</v>
       </c>
       <c r="B1766" t="s">
-        <v>2346</v>
+        <v>2340</v>
       </c>
       <c r="C1766" t="s">
-        <v>2347</v>
+        <v>2341</v>
       </c>
       <c r="D1766" t="s">
         <v>12</v>
@@ -72339,7 +72317,7 @@
         <v>13</v>
       </c>
       <c r="F1766" t="s">
-        <v>2345</v>
+        <v>2339</v>
       </c>
       <c r="G1766">
         <v>10002</v>
@@ -72348,7 +72326,7 @@
         <v>50</v>
       </c>
       <c r="I1766" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1766" t="s">
         <v>32</v>
@@ -72362,10 +72340,10 @@
         <v>1250</v>
       </c>
       <c r="B1767" t="s">
-        <v>2348</v>
+        <v>2342</v>
       </c>
       <c r="C1767" t="s">
-        <v>2338</v>
+        <v>2332</v>
       </c>
       <c r="D1767" t="s">
         <v>12</v>
@@ -72374,7 +72352,7 @@
         <v>13</v>
       </c>
       <c r="F1767" t="s">
-        <v>2349</v>
+        <v>2343</v>
       </c>
       <c r="G1767">
         <v>10002</v>
@@ -72383,7 +72361,7 @@
         <v>50</v>
       </c>
       <c r="I1767" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1767" t="s">
         <v>26</v>
@@ -72400,7 +72378,7 @@
         <v>234</v>
       </c>
       <c r="C1768" t="s">
-        <v>2350</v>
+        <v>2344</v>
       </c>
       <c r="D1768" t="s">
         <v>12</v>
@@ -72409,7 +72387,7 @@
         <v>13</v>
       </c>
       <c r="F1768" t="s">
-        <v>2349</v>
+        <v>2343</v>
       </c>
       <c r="G1768">
         <v>10002</v>
@@ -72418,7 +72396,7 @@
         <v>50</v>
       </c>
       <c r="I1768" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1768" t="s">
         <v>32</v>
@@ -72432,10 +72410,10 @@
         <v>1681</v>
       </c>
       <c r="B1769" t="s">
-        <v>2351</v>
+        <v>2345</v>
       </c>
       <c r="C1769" t="s">
-        <v>2351</v>
+        <v>2345</v>
       </c>
       <c r="D1769" t="s">
         <v>12</v>
@@ -72444,7 +72422,7 @@
         <v>13</v>
       </c>
       <c r="F1769" t="s">
-        <v>2352</v>
+        <v>2346</v>
       </c>
       <c r="G1769">
         <v>10001</v>
@@ -72453,7 +72431,7 @@
         <v>153</v>
       </c>
       <c r="I1769" t="s">
-        <v>2353</v>
+        <v>2347</v>
       </c>
       <c r="J1769" t="s">
         <v>17</v>
@@ -72467,10 +72445,10 @@
         <v>1269</v>
       </c>
       <c r="B1770" t="s">
-        <v>2354</v>
+        <v>2348</v>
       </c>
       <c r="C1770" t="s">
-        <v>2355</v>
+        <v>2349</v>
       </c>
       <c r="D1770" t="s">
         <v>12</v>
@@ -72479,7 +72457,7 @@
         <v>13</v>
       </c>
       <c r="F1770" t="s">
-        <v>2356</v>
+        <v>2350</v>
       </c>
       <c r="G1770">
         <v>10001</v>
@@ -72488,7 +72466,7 @@
         <v>153</v>
       </c>
       <c r="I1770" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
       <c r="J1770" t="s">
         <v>26</v>
@@ -72502,10 +72480,10 @@
         <v>1269</v>
       </c>
       <c r="B1771" t="s">
-        <v>2358</v>
+        <v>2352</v>
       </c>
       <c r="C1771" t="s">
-        <v>2359</v>
+        <v>2353</v>
       </c>
       <c r="D1771" t="s">
         <v>12</v>
@@ -72514,7 +72492,7 @@
         <v>13</v>
       </c>
       <c r="F1771" t="s">
-        <v>2360</v>
+        <v>2354</v>
       </c>
       <c r="G1771">
         <v>10001</v>
@@ -72523,7 +72501,7 @@
         <v>153</v>
       </c>
       <c r="I1771" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
       <c r="J1771" t="s">
         <v>32</v>
@@ -72537,10 +72515,10 @@
         <v>1269</v>
       </c>
       <c r="B1772" t="s">
-        <v>2361</v>
+        <v>2355</v>
       </c>
       <c r="C1772" t="s">
-        <v>2355</v>
+        <v>2349</v>
       </c>
       <c r="D1772" t="s">
         <v>12</v>
@@ -72549,7 +72527,7 @@
         <v>13</v>
       </c>
       <c r="F1772" t="s">
-        <v>2360</v>
+        <v>2354</v>
       </c>
       <c r="G1772">
         <v>10002</v>
@@ -72558,7 +72536,7 @@
         <v>50</v>
       </c>
       <c r="I1772" t="s">
-        <v>2362</v>
+        <v>2356</v>
       </c>
       <c r="J1772" t="s">
         <v>17</v>
@@ -72572,10 +72550,10 @@
         <v>1253</v>
       </c>
       <c r="B1773" t="s">
-        <v>2363</v>
+        <v>2357</v>
       </c>
       <c r="C1773" t="s">
-        <v>2363</v>
+        <v>2357</v>
       </c>
       <c r="D1773" t="s">
         <v>12</v>
@@ -72584,7 +72562,7 @@
         <v>13</v>
       </c>
       <c r="F1773" t="s">
-        <v>2364</v>
+        <v>2358</v>
       </c>
       <c r="G1773">
         <v>10002</v>
@@ -72593,7 +72571,7 @@
         <v>50</v>
       </c>
       <c r="I1773" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1773" t="s">
         <v>549</v>
@@ -72619,7 +72597,7 @@
         <v>13</v>
       </c>
       <c r="F1774" t="s">
-        <v>2365</v>
+        <v>2359</v>
       </c>
       <c r="G1774">
         <v>10002</v>
@@ -72628,7 +72606,7 @@
         <v>50</v>
       </c>
       <c r="I1774" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1774" t="s">
         <v>549</v>
@@ -72642,10 +72620,10 @@
         <v>1269</v>
       </c>
       <c r="B1775" t="s">
-        <v>2366</v>
+        <v>2360</v>
       </c>
       <c r="C1775" t="s">
-        <v>2367</v>
+        <v>2361</v>
       </c>
       <c r="D1775" t="s">
         <v>12</v>
@@ -72654,7 +72632,7 @@
         <v>13</v>
       </c>
       <c r="F1775" t="s">
-        <v>2368</v>
+        <v>2362</v>
       </c>
       <c r="G1775">
         <v>10001</v>
@@ -72663,7 +72641,7 @@
         <v>153</v>
       </c>
       <c r="I1775" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
       <c r="J1775" t="s">
         <v>549</v>
@@ -72677,10 +72655,10 @@
         <v>1269</v>
       </c>
       <c r="B1776" t="s">
-        <v>2369</v>
+        <v>2363</v>
       </c>
       <c r="C1776" t="s">
-        <v>2370</v>
+        <v>2364</v>
       </c>
       <c r="D1776" t="s">
         <v>12</v>
@@ -72689,7 +72667,7 @@
         <v>13</v>
       </c>
       <c r="F1776" t="s">
-        <v>2371</v>
+        <v>2365</v>
       </c>
       <c r="G1776">
         <v>10001</v>
@@ -72698,7 +72676,7 @@
         <v>153</v>
       </c>
       <c r="I1776" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
       <c r="J1776" t="s">
         <v>939</v>
@@ -72712,10 +72690,10 @@
         <v>1253</v>
       </c>
       <c r="B1777" t="s">
-        <v>2372</v>
+        <v>2366</v>
       </c>
       <c r="C1777" t="s">
-        <v>2372</v>
+        <v>2366</v>
       </c>
       <c r="D1777" t="s">
         <v>12</v>
@@ -72724,7 +72702,7 @@
         <v>13</v>
       </c>
       <c r="F1777" t="s">
-        <v>2373</v>
+        <v>2367</v>
       </c>
       <c r="G1777">
         <v>10002</v>
@@ -72733,7 +72711,7 @@
         <v>50</v>
       </c>
       <c r="I1777" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1777" t="s">
         <v>939</v>
@@ -72759,7 +72737,7 @@
         <v>13</v>
       </c>
       <c r="F1778" t="s">
-        <v>2374</v>
+        <v>2368</v>
       </c>
       <c r="G1778">
         <v>10002</v>
@@ -72768,7 +72746,7 @@
         <v>50</v>
       </c>
       <c r="I1778" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1778" t="s">
         <v>939</v>
@@ -72794,7 +72772,7 @@
         <v>13</v>
       </c>
       <c r="F1779" t="s">
-        <v>2375</v>
+        <v>2369</v>
       </c>
       <c r="G1779">
         <v>10002</v>
@@ -72803,7 +72781,7 @@
         <v>50</v>
       </c>
       <c r="I1779" t="s">
-        <v>2340</v>
+        <v>2334</v>
       </c>
       <c r="J1779" t="s">
         <v>990</v>
@@ -72817,10 +72795,10 @@
         <v>1283</v>
       </c>
       <c r="B1780" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="C1780" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
       <c r="D1780" t="s">
         <v>12</v>
@@ -72829,7 +72807,7 @@
         <v>13</v>
       </c>
       <c r="F1780" t="s">
-        <v>2378</v>
+        <v>2372</v>
       </c>
       <c r="G1780">
         <v>10002</v>
@@ -72838,7 +72816,7 @@
         <v>50</v>
       </c>
       <c r="I1780" t="s">
-        <v>2379</v>
+        <v>2373</v>
       </c>
       <c r="J1780" t="s">
         <v>26</v>
@@ -72852,10 +72830,10 @@
         <v>1284</v>
       </c>
       <c r="B1781" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="C1781" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
       <c r="D1781" t="s">
         <v>12</v>
@@ -72864,7 +72842,7 @@
         <v>13</v>
       </c>
       <c r="F1781" t="s">
-        <v>2378</v>
+        <v>2372</v>
       </c>
       <c r="G1781">
         <v>10002</v>
@@ -72873,7 +72851,7 @@
         <v>50</v>
       </c>
       <c r="I1781" t="s">
-        <v>2379</v>
+        <v>2373</v>
       </c>
       <c r="J1781" t="s">
         <v>32</v>
@@ -72887,10 +72865,10 @@
         <v>1126</v>
       </c>
       <c r="B1782" t="s">
-        <v>2380</v>
+        <v>2374</v>
       </c>
       <c r="C1782" t="s">
-        <v>2380</v>
+        <v>2374</v>
       </c>
       <c r="D1782" t="s">
         <v>12</v>
@@ -72899,7 +72877,7 @@
         <v>13</v>
       </c>
       <c r="F1782" t="s">
-        <v>2381</v>
+        <v>2375</v>
       </c>
       <c r="G1782">
         <v>10001</v>
@@ -72922,10 +72900,10 @@
         <v>1269</v>
       </c>
       <c r="B1783" t="s">
-        <v>2382</v>
+        <v>2376</v>
       </c>
       <c r="C1783" t="s">
-        <v>2383</v>
+        <v>2377</v>
       </c>
       <c r="D1783" t="s">
         <v>12</v>
@@ -72934,7 +72912,7 @@
         <v>13</v>
       </c>
       <c r="F1783" t="s">
-        <v>2384</v>
+        <v>2378</v>
       </c>
       <c r="G1783">
         <v>10001</v>
@@ -72943,7 +72921,7 @@
         <v>153</v>
       </c>
       <c r="I1783" t="s">
-        <v>2357</v>
+        <v>2351</v>
       </c>
       <c r="J1783" t="s">
         <v>990</v>
@@ -72957,10 +72935,10 @@
         <v>1260</v>
       </c>
       <c r="B1784" t="s">
-        <v>2385</v>
+        <v>2379</v>
       </c>
       <c r="C1784" t="s">
-        <v>2386</v>
+        <v>2380</v>
       </c>
       <c r="D1784" t="s">
         <v>12</v>
@@ -72969,7 +72947,7 @@
         <v>13</v>
       </c>
       <c r="F1784" t="s">
-        <v>2387</v>
+        <v>2381</v>
       </c>
       <c r="G1784">
         <v>10002</v>
@@ -72978,7 +72956,7 @@
         <v>50</v>
       </c>
       <c r="I1784" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1784" t="s">
         <v>17</v>
@@ -72992,10 +72970,10 @@
         <v>1260</v>
       </c>
       <c r="B1785" t="s">
-        <v>2389</v>
+        <v>2383</v>
       </c>
       <c r="C1785" t="s">
-        <v>2386</v>
+        <v>2380</v>
       </c>
       <c r="D1785" t="s">
         <v>12</v>
@@ -73004,7 +72982,7 @@
         <v>13</v>
       </c>
       <c r="F1785" t="s">
-        <v>2387</v>
+        <v>2381</v>
       </c>
       <c r="G1785">
         <v>10002</v>
@@ -73013,7 +72991,7 @@
         <v>50</v>
       </c>
       <c r="I1785" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1785" t="s">
         <v>26</v>
@@ -73027,10 +73005,10 @@
         <v>1260</v>
       </c>
       <c r="B1786" t="s">
-        <v>2390</v>
+        <v>2384</v>
       </c>
       <c r="C1786" t="s">
-        <v>2391</v>
+        <v>2385</v>
       </c>
       <c r="D1786" t="s">
         <v>12</v>
@@ -73039,7 +73017,7 @@
         <v>13</v>
       </c>
       <c r="F1786" t="s">
-        <v>2387</v>
+        <v>2381</v>
       </c>
       <c r="G1786">
         <v>10002</v>
@@ -73048,7 +73026,7 @@
         <v>50</v>
       </c>
       <c r="I1786" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1786" t="s">
         <v>32</v>
@@ -73062,10 +73040,10 @@
         <v>1282</v>
       </c>
       <c r="B1787" t="s">
-        <v>2376</v>
+        <v>2370</v>
       </c>
       <c r="C1787" t="s">
-        <v>2377</v>
+        <v>2371</v>
       </c>
       <c r="D1787" t="s">
         <v>12</v>
@@ -73074,7 +73052,7 @@
         <v>13</v>
       </c>
       <c r="F1787" t="s">
-        <v>2378</v>
+        <v>2372</v>
       </c>
       <c r="G1787">
         <v>10002</v>
@@ -73083,7 +73061,7 @@
         <v>50</v>
       </c>
       <c r="I1787" t="s">
-        <v>2379</v>
+        <v>2373</v>
       </c>
       <c r="J1787" t="s">
         <v>17</v>
@@ -73097,10 +73075,10 @@
         <v>1260</v>
       </c>
       <c r="B1788" t="s">
-        <v>2392</v>
+        <v>2386</v>
       </c>
       <c r="C1788" t="s">
-        <v>2392</v>
+        <v>2386</v>
       </c>
       <c r="D1788" t="s">
         <v>12</v>
@@ -73109,7 +73087,7 @@
         <v>13</v>
       </c>
       <c r="F1788" t="s">
-        <v>2393</v>
+        <v>2387</v>
       </c>
       <c r="G1788">
         <v>10002</v>
@@ -73118,7 +73096,7 @@
         <v>50</v>
       </c>
       <c r="I1788" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1788" t="s">
         <v>549</v>
@@ -73132,10 +73110,10 @@
         <v>1260</v>
       </c>
       <c r="B1789" t="s">
-        <v>2394</v>
+        <v>2388</v>
       </c>
       <c r="C1789" t="s">
-        <v>2394</v>
+        <v>2388</v>
       </c>
       <c r="D1789" t="s">
         <v>12</v>
@@ -73144,7 +73122,7 @@
         <v>13</v>
       </c>
       <c r="F1789" t="s">
-        <v>2395</v>
+        <v>2389</v>
       </c>
       <c r="G1789">
         <v>10002</v>
@@ -73153,7 +73131,7 @@
         <v>50</v>
       </c>
       <c r="I1789" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1789" t="s">
         <v>939</v>
@@ -73167,10 +73145,10 @@
         <v>1260</v>
       </c>
       <c r="B1790" t="s">
-        <v>2396</v>
+        <v>2390</v>
       </c>
       <c r="C1790" t="s">
-        <v>2396</v>
+        <v>2390</v>
       </c>
       <c r="D1790" t="s">
         <v>12</v>
@@ -73179,7 +73157,7 @@
         <v>13</v>
       </c>
       <c r="F1790" t="s">
-        <v>2397</v>
+        <v>2391</v>
       </c>
       <c r="G1790">
         <v>10002</v>
@@ -73188,7 +73166,7 @@
         <v>50</v>
       </c>
       <c r="I1790" t="s">
-        <v>2388</v>
+        <v>2382</v>
       </c>
       <c r="J1790" t="s">
         <v>990</v>
@@ -73202,10 +73180,10 @@
         <v>1253</v>
       </c>
       <c r="B1791" t="s">
-        <v>2398</v>
+        <v>2392</v>
       </c>
       <c r="C1791" t="s">
-        <v>2398</v>
+        <v>2392</v>
       </c>
       <c r="D1791" t="s">
         <v>12</v>
@@ -73214,7 +73192,7 @@
         <v>13</v>
       </c>
       <c r="F1791" t="s">
-        <v>2399</v>
+        <v>2393</v>
       </c>
       <c r="G1791">
         <v>10002</v>
@@ -73223,7 +73201,7 @@
         <v>50</v>
       </c>
       <c r="I1791" t="s">
-        <v>2326</v>
+        <v>2320</v>
       </c>
       <c r="J1791" t="s">
         <v>990</v>
@@ -73234,13 +73212,13 @@
     </row>
     <row r="1792" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1792" t="s">
-        <v>2400</v>
+        <v>2394</v>
       </c>
       <c r="B1792" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="C1792" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="D1792" t="s">
         <v>201</v>
@@ -73249,7 +73227,7 @@
         <v>13</v>
       </c>
       <c r="F1792" t="s">
-        <v>2402</v>
+        <v>2396</v>
       </c>
       <c r="G1792">
         <v>10003</v>
@@ -73269,13 +73247,13 @@
     </row>
     <row r="1793" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1793" t="s">
-        <v>2403</v>
+        <v>2397</v>
       </c>
       <c r="B1793" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="C1793" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="D1793" t="s">
         <v>201</v>
@@ -73284,7 +73262,7 @@
         <v>13</v>
       </c>
       <c r="F1793" t="s">
-        <v>2404</v>
+        <v>2398</v>
       </c>
       <c r="G1793">
         <v>10003</v>
@@ -73307,10 +73285,10 @@
         <v>1131</v>
       </c>
       <c r="B1794" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="C1794" t="s">
-        <v>2401</v>
+        <v>2395</v>
       </c>
       <c r="D1794" t="s">
         <v>201</v>
@@ -73319,7 +73297,7 @@
         <v>13</v>
       </c>
       <c r="F1794" t="s">
-        <v>2405</v>
+        <v>2399</v>
       </c>
       <c r="G1794">
         <v>10003</v>
@@ -73342,10 +73320,10 @@
         <v>1101</v>
       </c>
       <c r="B1795" t="s">
-        <v>2406</v>
+        <v>2400</v>
       </c>
       <c r="C1795" t="s">
-        <v>2406</v>
+        <v>2400</v>
       </c>
       <c r="D1795" t="s">
         <v>12</v>
@@ -73354,7 +73332,7 @@
         <v>13</v>
       </c>
       <c r="F1795" t="s">
-        <v>2407</v>
+        <v>2401</v>
       </c>
       <c r="G1795">
         <v>10004</v>
@@ -73363,7 +73341,7 @@
         <v>31</v>
       </c>
       <c r="I1795" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1795" t="s">
         <v>32</v>
@@ -73377,10 +73355,10 @@
         <v>1101</v>
       </c>
       <c r="B1796" t="s">
-        <v>2409</v>
+        <v>2403</v>
       </c>
       <c r="C1796" t="s">
-        <v>2409</v>
+        <v>2403</v>
       </c>
       <c r="D1796" t="s">
         <v>12</v>
@@ -73389,7 +73367,7 @@
         <v>13</v>
       </c>
       <c r="F1796" t="s">
-        <v>2410</v>
+        <v>2404</v>
       </c>
       <c r="G1796">
         <v>10004</v>
@@ -73398,7 +73376,7 @@
         <v>25</v>
       </c>
       <c r="I1796" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1796" t="s">
         <v>26</v>
@@ -73424,7 +73402,7 @@
         <v>13</v>
       </c>
       <c r="F1797" t="s">
-        <v>2411</v>
+        <v>2405</v>
       </c>
       <c r="G1797">
         <v>10004</v>
@@ -73433,7 +73411,7 @@
         <v>1060</v>
       </c>
       <c r="I1797" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1797" t="s">
         <v>939</v>
@@ -73459,7 +73437,7 @@
         <v>13</v>
       </c>
       <c r="F1798" t="s">
-        <v>2412</v>
+        <v>2406</v>
       </c>
       <c r="G1798">
         <v>10004</v>
@@ -73468,7 +73446,7 @@
         <v>548</v>
       </c>
       <c r="I1798" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1798" t="s">
         <v>549</v>
@@ -73494,7 +73472,7 @@
         <v>13</v>
       </c>
       <c r="F1799" t="s">
-        <v>2413</v>
+        <v>2407</v>
       </c>
       <c r="G1799">
         <v>10004</v>
@@ -73503,7 +73481,7 @@
         <v>1283</v>
       </c>
       <c r="I1799" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1799" t="s">
         <v>990</v>
@@ -73517,10 +73495,10 @@
         <v>1683</v>
       </c>
       <c r="B1800" t="s">
-        <v>2414</v>
+        <v>2408</v>
       </c>
       <c r="C1800" t="s">
-        <v>2335</v>
+        <v>2329</v>
       </c>
       <c r="D1800" t="s">
         <v>12</v>
@@ -73529,7 +73507,7 @@
         <v>13</v>
       </c>
       <c r="F1800" t="s">
-        <v>2336</v>
+        <v>2330</v>
       </c>
       <c r="G1800">
         <v>10002</v>
@@ -73538,7 +73516,7 @@
         <v>50</v>
       </c>
       <c r="I1800" t="s">
-        <v>2415</v>
+        <v>2409</v>
       </c>
       <c r="J1800" t="s">
         <v>17</v>
@@ -73552,10 +73530,10 @@
         <v>1124</v>
       </c>
       <c r="B1801" t="s">
-        <v>2416</v>
+        <v>2410</v>
       </c>
       <c r="C1801" t="s">
-        <v>2416</v>
+        <v>2410</v>
       </c>
       <c r="D1801" t="s">
         <v>12</v>
@@ -73564,7 +73542,7 @@
         <v>13</v>
       </c>
       <c r="F1801" t="s">
-        <v>2417</v>
+        <v>2411</v>
       </c>
       <c r="G1801">
         <v>10001</v>
@@ -73587,10 +73565,10 @@
         <v>1125</v>
       </c>
       <c r="B1802" t="s">
-        <v>2418</v>
+        <v>2412</v>
       </c>
       <c r="C1802" t="s">
-        <v>2418</v>
+        <v>2412</v>
       </c>
       <c r="D1802" t="s">
         <v>12</v>
@@ -73599,7 +73577,7 @@
         <v>13</v>
       </c>
       <c r="F1802" t="s">
-        <v>2419</v>
+        <v>2413</v>
       </c>
       <c r="G1802">
         <v>10001</v>
@@ -73619,13 +73597,13 @@
     </row>
     <row r="1803" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1803" t="s">
-        <v>2420</v>
+        <v>2414</v>
       </c>
       <c r="B1803" t="s">
-        <v>2421</v>
+        <v>2415</v>
       </c>
       <c r="C1803" t="s">
-        <v>2421</v>
+        <v>2415</v>
       </c>
       <c r="D1803" t="s">
         <v>12</v>
@@ -73634,7 +73612,7 @@
         <v>13</v>
       </c>
       <c r="F1803" t="s">
-        <v>2422</v>
+        <v>2416</v>
       </c>
       <c r="G1803">
         <v>10001</v>
@@ -73654,13 +73632,13 @@
     </row>
     <row r="1804" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1804" t="s">
-        <v>2423</v>
+        <v>2417</v>
       </c>
       <c r="B1804" t="s">
-        <v>2424</v>
+        <v>2418</v>
       </c>
       <c r="C1804" t="s">
-        <v>2424</v>
+        <v>2418</v>
       </c>
       <c r="D1804" t="s">
         <v>12</v>
@@ -73669,7 +73647,7 @@
         <v>13</v>
       </c>
       <c r="F1804" t="s">
-        <v>2422</v>
+        <v>2416</v>
       </c>
       <c r="G1804">
         <v>10001</v>
@@ -73689,13 +73667,13 @@
     </row>
     <row r="1805" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1805" t="s">
-        <v>2425</v>
+        <v>2419</v>
       </c>
       <c r="B1805" t="s">
-        <v>2331</v>
+        <v>2325</v>
       </c>
       <c r="C1805" t="s">
-        <v>2331</v>
+        <v>2325</v>
       </c>
       <c r="D1805" t="s">
         <v>12</v>
@@ -73704,7 +73682,7 @@
         <v>13</v>
       </c>
       <c r="F1805" t="s">
-        <v>2426</v>
+        <v>2420</v>
       </c>
       <c r="G1805">
         <v>10001</v>
@@ -73727,10 +73705,10 @@
         <v>1154</v>
       </c>
       <c r="B1806" t="s">
-        <v>2427</v>
+        <v>2421</v>
       </c>
       <c r="C1806" t="s">
-        <v>2427</v>
+        <v>2421</v>
       </c>
       <c r="D1806" t="s">
         <v>12</v>
@@ -73739,7 +73717,7 @@
         <v>13</v>
       </c>
       <c r="F1806" t="s">
-        <v>2428</v>
+        <v>2422</v>
       </c>
       <c r="G1806">
         <v>10001</v>
@@ -73762,10 +73740,10 @@
         <v>1101</v>
       </c>
       <c r="B1807" t="s">
-        <v>2429</v>
+        <v>2423</v>
       </c>
       <c r="C1807" t="s">
-        <v>2429</v>
+        <v>2423</v>
       </c>
       <c r="D1807" t="s">
         <v>12</v>
@@ -73774,7 +73752,7 @@
         <v>13</v>
       </c>
       <c r="F1807" t="s">
-        <v>2430</v>
+        <v>2424</v>
       </c>
       <c r="G1807">
         <v>10004</v>
@@ -73783,7 +73761,7 @@
         <v>15</v>
       </c>
       <c r="I1807" t="s">
-        <v>2408</v>
+        <v>2402</v>
       </c>
       <c r="J1807" t="s">
         <v>17</v>
@@ -73792,15 +73770,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1808" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="1808" spans="1:11" ht="35.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1808" t="s">
-        <v>2437</v>
+        <v>2431</v>
       </c>
       <c r="B1808" t="s">
-        <v>2438</v>
+        <v>2432</v>
       </c>
       <c r="C1808" t="s">
-        <v>2438</v>
+        <v>2432</v>
       </c>
       <c r="D1808" t="s">
         <v>12</v>
@@ -73809,7 +73787,7 @@
         <v>13</v>
       </c>
       <c r="F1808" s="1" t="s">
-        <v>2439</v>
+        <v>2433</v>
       </c>
       <c r="G1808">
         <v>10003</v>
@@ -73818,7 +73796,7 @@
         <v>58</v>
       </c>
       <c r="I1808" t="s">
-        <v>2440</v>
+        <v>2434</v>
       </c>
       <c r="J1808" t="s">
         <v>17</v>
@@ -73827,15 +73805,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1809" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="1809" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1809" t="s">
-        <v>2441</v>
+        <v>2435</v>
       </c>
       <c r="B1809" t="s">
-        <v>2442</v>
+        <v>2436</v>
       </c>
       <c r="C1809" t="s">
-        <v>2442</v>
+        <v>2436</v>
       </c>
       <c r="D1809" t="s">
         <v>12</v>
@@ -73844,7 +73822,7 @@
         <v>13</v>
       </c>
       <c r="F1809" s="1" t="s">
-        <v>2443</v>
+        <v>2437</v>
       </c>
       <c r="G1809">
         <v>10003</v>
@@ -73853,7 +73831,7 @@
         <v>58</v>
       </c>
       <c r="I1809" t="s">
-        <v>2440</v>
+        <v>2434</v>
       </c>
       <c r="J1809" t="s">
         <v>17</v>
@@ -73864,10 +73842,17 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:K1807" xr:uid="{5198E219-C078-4DCC-B3A9-17881A6ADC0B}">
+  <autoFilter ref="A1:K1809" xr:uid="{5198E219-C078-4DCC-B3A9-17881A6ADC0B}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Template for UIN Reactivate Email"/>
+        <filter val="Template for Supervisor Reject Email"/>
+        <filter val="Template for Supervisor Reject Email Subject"/>
+        <filter val="Template for Supervisor Reject SMS"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="eng"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Changes in template code
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A86664-853D-4805-B751-5CDE69C640BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D4AA5-7239-4E08-8668-9A6834996CC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16305" uniqueCount="2459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16305" uniqueCount="2460">
   <si>
     <t>id</t>
   </si>
@@ -10256,6 +10256,9 @@
 Your event id is #$eventId. &lt;br&gt;
 Log in to the official website $trackServiceRequestLink for further details. &lt;br&gt;</t>
   </si>
+  <si>
+    <t>Regproc-Renewal-Email</t>
+  </si>
 </sst>
 </file>
 
@@ -10599,14 +10602,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1809"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A1797" workbookViewId="0">
+      <selection activeCell="I1808" sqref="I1808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="6" max="6" width="56.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -73909,7 +73913,7 @@
         <v>57</v>
       </c>
       <c r="I1809" t="s">
-        <v>2388</v>
+        <v>2459</v>
       </c>
       <c r="J1809" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
template code changes code in template and template_type file (#9)
* Updated renewal template type for SMS and email

* updated al template

* Updated template.xlsx file for reject mail/sms

* Updated template.xlsx file reject sms/mail/sub

* changes for placeholder name to givenname and surname

* Changes in template code
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nira_dev\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A86664-853D-4805-B751-5CDE69C640BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D4AA5-7239-4E08-8668-9A6834996CC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16305" uniqueCount="2459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16305" uniqueCount="2460">
   <si>
     <t>id</t>
   </si>
@@ -10256,6 +10256,9 @@
 Your event id is #$eventId. &lt;br&gt;
 Log in to the official website $trackServiceRequestLink for further details. &lt;br&gt;</t>
   </si>
+  <si>
+    <t>Regproc-Renewal-Email</t>
+  </si>
 </sst>
 </file>
 
@@ -10599,14 +10602,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1809"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A1797" workbookViewId="0">
+      <selection activeCell="I1808" sqref="I1808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="6" max="6" width="56.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -73909,7 +73913,7 @@
         <v>57</v>
       </c>
       <c r="I1809" t="s">
-        <v>2388</v>
+        <v>2459</v>
       </c>
       <c r="J1809" t="s">
         <v>17</v>

</xml_diff>